<commit_message>
Lots of changes adding functionality.  Closes #17, closes #18, and closes #22.
</commit_message>
<xml_diff>
--- a/Support/Signal List.xlsx
+++ b/Support/Signal List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9645" windowHeight="3870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9648" windowHeight="3876"/>
   </bookViews>
   <sheets>
     <sheet name="DAQ Signals All" sheetId="11" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1688" uniqueCount="842">
   <si>
     <t>Speaker Out</t>
   </si>
@@ -3570,6 +3570,102 @@
   </si>
   <si>
     <t>Blue1 Gain</t>
+  </si>
+  <si>
+    <t>Inlet LED</t>
+  </si>
+  <si>
+    <t>P2.0</t>
+  </si>
+  <si>
+    <t>P2.1</t>
+  </si>
+  <si>
+    <t>P2.2</t>
+  </si>
+  <si>
+    <t>P2.3</t>
+  </si>
+  <si>
+    <t>P2.4</t>
+  </si>
+  <si>
+    <t>P2.5</t>
+  </si>
+  <si>
+    <t>P2.6</t>
+  </si>
+  <si>
+    <t>P2.7</t>
+  </si>
+  <si>
+    <t>Filter LED</t>
+  </si>
+  <si>
+    <t>Denuder LED</t>
+  </si>
+  <si>
+    <t>O3 LED</t>
+  </si>
+  <si>
+    <t>Spk LED</t>
+  </si>
+  <si>
+    <t>405 LED</t>
+  </si>
+  <si>
+    <t>515 LED</t>
+  </si>
+  <si>
+    <t>660 LED</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Heartbeat</t>
+  </si>
+  <si>
+    <t>Sample Pump Enable</t>
+  </si>
+  <si>
+    <t>17,18</t>
+  </si>
+  <si>
+    <t>47,13</t>
+  </si>
+  <si>
+    <t>37,4</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>45,12</t>
+  </si>
+  <si>
+    <t>46,12</t>
+  </si>
+  <si>
+    <t>2,4</t>
+  </si>
+  <si>
+    <t>1,35</t>
+  </si>
+  <si>
+    <t>39,4</t>
+  </si>
+  <si>
+    <t>49,15</t>
+  </si>
+  <si>
+    <t>19,53</t>
+  </si>
+  <si>
+    <t>Ozone DO</t>
+  </si>
+  <si>
+    <t>ctr0</t>
   </si>
 </sst>
 </file>
@@ -3662,6 +3758,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3670,15 +3775,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3960,27 +4056,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="75.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="75.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>713</v>
       </c>
@@ -4012,7 +4108,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>312</v>
       </c>
@@ -4044,7 +4140,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
@@ -4073,7 +4169,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
@@ -4102,7 +4198,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
@@ -4131,7 +4227,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -4160,7 +4256,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
@@ -4189,7 +4285,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
@@ -4218,7 +4314,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
@@ -4247,7 +4343,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>35</v>
       </c>
@@ -4276,7 +4372,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>37</v>
       </c>
@@ -4305,7 +4401,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
@@ -4334,7 +4430,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>41</v>
       </c>
@@ -4363,7 +4459,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>51</v>
       </c>
@@ -4392,7 +4488,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>53</v>
       </c>
@@ -4421,7 +4517,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>54</v>
       </c>
@@ -4450,7 +4546,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>55</v>
       </c>
@@ -4479,7 +4575,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>56</v>
       </c>
@@ -4508,7 +4604,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>170</v>
       </c>
@@ -4535,7 +4631,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>171</v>
       </c>
@@ -4562,7 +4658,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>172</v>
       </c>
@@ -4589,7 +4685,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>173</v>
       </c>
@@ -4616,7 +4712,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>174</v>
       </c>
@@ -4643,7 +4739,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>73</v>
       </c>
@@ -4670,7 +4766,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>74</v>
       </c>
@@ -4697,7 +4793,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>75</v>
       </c>
@@ -4724,7 +4820,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>76</v>
       </c>
@@ -4751,7 +4847,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>77</v>
       </c>
@@ -4778,7 +4874,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>80</v>
       </c>
@@ -4805,7 +4901,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>81</v>
       </c>
@@ -4832,7 +4928,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>83</v>
       </c>
@@ -4859,7 +4955,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>84</v>
       </c>
@@ -4886,7 +4982,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>85</v>
       </c>
@@ -4913,7 +5009,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>94</v>
       </c>
@@ -4940,7 +5036,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
         <v>95</v>
       </c>
@@ -4967,7 +5063,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
         <v>96</v>
       </c>
@@ -4994,7 +5090,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>97</v>
       </c>
@@ -5021,7 +5117,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>98</v>
       </c>
@@ -5048,7 +5144,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
         <v>104</v>
       </c>
@@ -5075,7 +5171,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B40" s="3" t="s">
         <v>105</v>
       </c>
@@ -5102,7 +5198,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B41" s="3" t="s">
         <v>106</v>
       </c>
@@ -5129,7 +5225,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="s">
         <v>107</v>
       </c>
@@ -5156,7 +5252,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
         <v>108</v>
       </c>
@@ -5183,91 +5279,96 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="19" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="17" t="s">
         <v>704</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="E44" s="1"/>
+      <c r="E44" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="F44" s="1">
         <v>0</v>
       </c>
-      <c r="G44" s="20">
+      <c r="G44" s="18">
         <v>6225</v>
       </c>
-      <c r="H44" s="20" t="s">
+      <c r="H44" s="18" t="s">
         <v>114</v>
       </c>
       <c r="I44" s="1">
         <v>6</v>
       </c>
-      <c r="J44" s="18" t="s">
+      <c r="J44" s="21" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="19"/>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B45" s="17"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="E45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>829</v>
+      </c>
       <c r="F45" s="1">
         <v>0</v>
       </c>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
       <c r="I45" s="1">
         <v>6</v>
       </c>
-      <c r="J45" s="18"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J45" s="21"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>411</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="19" t="s">
         <v>797</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>697</v>
       </c>
+      <c r="E46" s="1"/>
       <c r="F46" s="1">
         <v>0</v>
       </c>
-      <c r="G46" s="20">
+      <c r="G46" s="18">
         <v>6225</v>
       </c>
-      <c r="H46" s="20" t="s">
+      <c r="H46" s="18" t="s">
         <v>114</v>
       </c>
       <c r="I46" s="1">
         <v>7</v>
       </c>
-      <c r="J46" s="17" t="s">
+      <c r="J46" s="20" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="16"/>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B47" s="19"/>
       <c r="D47" s="1" t="s">
         <v>698</v>
       </c>
       <c r="F47" s="1">
         <v>0</v>
       </c>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
       <c r="I47" s="1">
         <v>7</v>
       </c>
-      <c r="J47" s="17"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="16" t="s">
+      <c r="J47" s="20"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B48" s="19" t="s">
         <v>799</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -5281,12 +5382,12 @@
       <c r="I48" s="1">
         <v>7</v>
       </c>
-      <c r="J48" s="17" t="s">
+      <c r="J48" s="20" t="s">
         <v>803</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="16"/>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B49" s="19"/>
       <c r="D49" s="1" t="s">
         <v>801</v>
       </c>
@@ -5298,10 +5399,10 @@
       <c r="I49" s="1">
         <v>7</v>
       </c>
-      <c r="J49" s="17"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="16" t="s">
+      <c r="J49" s="20"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B50" s="19" t="s">
         <v>798</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -5310,36 +5411,36 @@
       <c r="F50" s="1">
         <v>0</v>
       </c>
-      <c r="G50" s="20">
+      <c r="G50" s="18">
         <v>6225</v>
       </c>
-      <c r="H50" s="20" t="s">
+      <c r="H50" s="18" t="s">
         <v>114</v>
       </c>
       <c r="I50" s="1">
         <v>7</v>
       </c>
-      <c r="J50" s="17" t="s">
+      <c r="J50" s="20" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="16"/>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B51" s="19"/>
       <c r="D51" s="1" t="s">
         <v>705</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
       </c>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
       <c r="I51" s="1">
         <v>7</v>
       </c>
-      <c r="J51" s="17"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="16" t="s">
+      <c r="J51" s="20"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B52" s="19" t="s">
         <v>802</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -5353,12 +5454,12 @@
       <c r="I52" s="1">
         <v>7</v>
       </c>
-      <c r="J52" s="17" t="s">
+      <c r="J52" s="20" t="s">
         <v>804</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="16"/>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B53" s="19"/>
       <c r="D53" s="1" t="s">
         <v>806</v>
       </c>
@@ -5370,9 +5471,9 @@
       <c r="I53" s="1">
         <v>7</v>
       </c>
-      <c r="J53" s="17"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J53" s="20"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>707</v>
       </c>
@@ -5395,138 +5496,130 @@
         <v>794</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>266</v>
-      </c>
-      <c r="B55" s="19" t="s">
-        <v>719</v>
-      </c>
-      <c r="C55" s="1"/>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>810</v>
+      </c>
       <c r="D55" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>175</v>
+        <v>811</v>
+      </c>
+      <c r="E55" t="s">
+        <v>831</v>
       </c>
       <c r="F55" s="1">
         <v>0</v>
       </c>
       <c r="G55" s="1">
-        <v>6124</v>
-      </c>
-      <c r="H55" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I55" s="1">
-        <v>3</v>
-      </c>
-      <c r="J55" s="3" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="19"/>
-      <c r="C56" s="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>819</v>
+      </c>
       <c r="D56" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>231</v>
+        <v>812</v>
+      </c>
+      <c r="E56" t="s">
+        <v>832</v>
       </c>
       <c r="F56" s="1">
         <v>0</v>
       </c>
       <c r="G56" s="1">
-        <v>6124</v>
-      </c>
-      <c r="H56" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I56" s="1">
-        <v>3</v>
-      </c>
-      <c r="J56" s="3" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="19"/>
-      <c r="C57" s="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>820</v>
+      </c>
       <c r="D57" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>177</v>
+        <v>813</v>
+      </c>
+      <c r="E57" t="s">
+        <v>833</v>
       </c>
       <c r="F57" s="1">
         <v>0</v>
       </c>
       <c r="G57" s="1">
-        <v>6124</v>
-      </c>
-      <c r="H57" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I57" s="1">
-        <v>3</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B58" s="19"/>
-      <c r="C58" s="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>821</v>
+      </c>
       <c r="D58" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>232</v>
+        <v>814</v>
+      </c>
+      <c r="E58" t="s">
+        <v>834</v>
       </c>
       <c r="F58" s="1">
         <v>0</v>
       </c>
       <c r="G58" s="1">
-        <v>6124</v>
-      </c>
-      <c r="H58" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I58" s="1">
-        <v>3</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B59" s="3" t="s">
-        <v>720</v>
-      </c>
-      <c r="C59" s="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>822</v>
+      </c>
       <c r="D59" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>175</v>
+        <v>815</v>
+      </c>
+      <c r="E59" t="s">
+        <v>835</v>
       </c>
       <c r="F59" s="1">
         <v>0</v>
       </c>
       <c r="G59" s="1">
-        <v>6132</v>
-      </c>
-      <c r="H59" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I59" s="1">
-        <v>5</v>
-      </c>
-      <c r="J59" s="3" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B60" s="3" t="s">
-        <v>721</v>
-      </c>
-      <c r="C60" s="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>823</v>
+      </c>
       <c r="D60" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>160</v>
+        <v>816</v>
+      </c>
+      <c r="E60" t="s">
+        <v>233</v>
       </c>
       <c r="F60" s="1">
         <v>0</v>
@@ -5534,24 +5627,22 @@
       <c r="G60" s="1">
         <v>6225</v>
       </c>
-      <c r="H60" s="1"/>
+      <c r="H60" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I60" s="1">
-        <v>8</v>
-      </c>
-      <c r="J60" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B61" s="3" t="s">
-        <v>722</v>
-      </c>
-      <c r="C61" s="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>824</v>
+      </c>
       <c r="D61" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>233</v>
+        <v>817</v>
+      </c>
+      <c r="E61" t="s">
+        <v>836</v>
       </c>
       <c r="F61" s="1">
         <v>0</v>
@@ -5559,242 +5650,514 @@
       <c r="G61" s="1">
         <v>6225</v>
       </c>
-      <c r="H61" s="1"/>
+      <c r="H61" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I61" s="1">
-        <v>8</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B62" s="19" t="s">
-        <v>723</v>
-      </c>
-      <c r="C62" s="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>825</v>
+      </c>
       <c r="D62" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>111</v>
+        <v>818</v>
+      </c>
+      <c r="E62" t="s">
+        <v>837</v>
+      </c>
+      <c r="F62" s="1">
+        <v>0</v>
       </c>
       <c r="G62" s="1">
-        <v>6704</v>
-      </c>
-      <c r="H62" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I62" s="1">
         <v>6</v>
       </c>
-      <c r="J62" s="3"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B63" s="19"/>
-      <c r="C63" s="1"/>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>826</v>
+      </c>
       <c r="D63" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>111</v>
+        <v>703</v>
+      </c>
+      <c r="E63" t="s">
+        <v>838</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0</v>
       </c>
       <c r="G63" s="1">
-        <v>6704</v>
-      </c>
-      <c r="H63" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I63" s="1">
         <v>6</v>
       </c>
-      <c r="J63" s="3"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B64" s="19"/>
-      <c r="C64" s="1"/>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>827</v>
+      </c>
       <c r="D64" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>111</v>
+        <v>705</v>
+      </c>
+      <c r="E64" t="s">
+        <v>830</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0</v>
       </c>
       <c r="G64" s="1">
-        <v>6704</v>
-      </c>
-      <c r="H64" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I64" s="1">
         <v>6</v>
       </c>
-      <c r="J64" s="3"/>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="19"/>
-      <c r="C65" s="1"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>828</v>
+      </c>
       <c r="D65" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>111</v>
+        <v>708</v>
+      </c>
+      <c r="E65" t="s">
+        <v>839</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0</v>
       </c>
       <c r="G65" s="1">
-        <v>6704</v>
-      </c>
-      <c r="H65" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I65" s="1">
         <v>6</v>
       </c>
-      <c r="J65" s="3"/>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="19"/>
-      <c r="C66" s="1"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>840</v>
+      </c>
       <c r="D66" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G66" s="1">
-        <v>6704</v>
+        <v>841</v>
       </c>
       <c r="H66" s="1"/>
-      <c r="I66" s="1">
-        <v>6</v>
-      </c>
-      <c r="J66" s="3"/>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" s="3" t="s">
-        <v>724</v>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>266</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>719</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="E67" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F67" s="1">
+        <v>0</v>
+      </c>
       <c r="G67" s="1">
-        <v>6225</v>
+        <v>6124</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="19" t="s">
-        <v>725</v>
-      </c>
+        <v>717</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B68" s="17"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="E68" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="F68" s="1">
         <v>0</v>
       </c>
       <c r="G68" s="1">
-        <v>6225</v>
+        <v>6124</v>
       </c>
       <c r="H68" s="1"/>
       <c r="I68" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" s="19"/>
+        <v>718</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B69" s="17"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>703</v>
-      </c>
-      <c r="E69" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="F69" s="1">
         <v>0</v>
       </c>
       <c r="G69" s="1">
-        <v>6225</v>
+        <v>6124</v>
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" s="21" t="s">
-        <v>807</v>
-      </c>
+        <v>715</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B70" s="17"/>
+      <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1">
+        <v>6124</v>
+      </c>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1">
+        <v>3</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B71" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F71" s="1">
+        <v>0</v>
+      </c>
+      <c r="G71" s="1">
+        <v>6132</v>
+      </c>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1">
         <v>5</v>
       </c>
-      <c r="G70" s="1">
-        <v>6704</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" s="21" t="s">
-        <v>808</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G71" s="1">
-        <v>6704</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J71" s="3" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B72" s="3" t="s">
-        <v>809</v>
+        <v>721</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F72" s="1">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1">
+        <v>6225</v>
+      </c>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1">
+        <v>8</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B73" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F73" s="1">
+        <v>0</v>
+      </c>
+      <c r="G73" s="1">
+        <v>6225</v>
+      </c>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1">
+        <v>8</v>
+      </c>
+      <c r="J73" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B74" s="17" t="s">
+        <v>723</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G74" s="1">
+        <v>6704</v>
+      </c>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1">
+        <v>6</v>
+      </c>
+      <c r="J74" s="3"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B75" s="17"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G75" s="1">
+        <v>6704</v>
+      </c>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1">
+        <v>6</v>
+      </c>
+      <c r="J75" s="3"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B76" s="17"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G76" s="1">
+        <v>6704</v>
+      </c>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1">
+        <v>6</v>
+      </c>
+      <c r="J76" s="3"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B77" s="17"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G77" s="1">
+        <v>6704</v>
+      </c>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1">
+        <v>6</v>
+      </c>
+      <c r="J77" s="3"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B78" s="17"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G78" s="1">
+        <v>6704</v>
+      </c>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1">
+        <v>6</v>
+      </c>
+      <c r="J78" s="3"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B79" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="E79" s="1"/>
+      <c r="G79" s="1">
+        <v>6225</v>
+      </c>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1">
+        <v>8</v>
+      </c>
+      <c r="J79" s="3" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B80" s="17" t="s">
+        <v>725</v>
+      </c>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1">
+        <v>6225</v>
+      </c>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1">
+        <v>8</v>
+      </c>
+      <c r="J80" s="3" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B81" s="17"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1">
+        <v>0</v>
+      </c>
+      <c r="G81" s="1">
+        <v>6225</v>
+      </c>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1">
+        <v>8</v>
+      </c>
+      <c r="J81" s="3" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B82" s="16" t="s">
+        <v>807</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G82" s="1">
+        <v>6704</v>
+      </c>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B83" s="16" t="s">
+        <v>808</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G83" s="1">
+        <v>6704</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B84" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E72" s="1"/>
-      <c r="G72" s="1">
+      <c r="E84" s="1"/>
+      <c r="G84" s="1">
         <v>6704</v>
       </c>
-      <c r="H72" s="1"/>
+      <c r="H84" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="H46:H47"/>
+    <mergeCell ref="H50:H51"/>
     <mergeCell ref="J48:J49"/>
     <mergeCell ref="J52:J53"/>
     <mergeCell ref="J50:J51"/>
     <mergeCell ref="J44:J45"/>
     <mergeCell ref="J46:J47"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="H46:H47"/>
-    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="B74:B78"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B52:B53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5809,12 +6172,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>312</v>
       </c>
@@ -5825,7 +6188,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>660</v>
       </c>
@@ -5833,7 +6196,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>509</v>
       </c>
@@ -5841,7 +6204,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>511</v>
       </c>
@@ -5849,7 +6212,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>512</v>
       </c>
@@ -5857,7 +6220,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>661</v>
       </c>
@@ -5865,7 +6228,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>662</v>
       </c>
@@ -5873,7 +6236,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>663</v>
       </c>
@@ -5881,7 +6244,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>664</v>
       </c>
@@ -5889,7 +6252,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>665</v>
       </c>
@@ -5897,7 +6260,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>666</v>
       </c>
@@ -5905,7 +6268,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>667</v>
       </c>
@@ -5913,7 +6276,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>668</v>
       </c>
@@ -5921,7 +6284,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>669</v>
       </c>
@@ -5929,7 +6292,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>670</v>
       </c>
@@ -5937,7 +6300,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>671</v>
       </c>
@@ -5945,7 +6308,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>266</v>
       </c>
@@ -5956,7 +6319,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>572</v>
       </c>
@@ -5964,7 +6327,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>672</v>
       </c>
@@ -5972,7 +6335,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>411</v>
       </c>
@@ -5983,7 +6346,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>674</v>
       </c>
@@ -5991,7 +6354,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>675</v>
       </c>
@@ -5999,7 +6362,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>676</v>
       </c>
@@ -6007,7 +6370,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>684</v>
       </c>
@@ -6015,7 +6378,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>677</v>
       </c>
@@ -6023,7 +6386,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>515</v>
       </c>
@@ -6031,22 +6394,22 @@
         <v>679</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>402</v>
       </c>
@@ -6054,17 +6417,17 @@
         <v>680</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>683</v>
       </c>
@@ -6072,17 +6435,17 @@
         <v>483</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>521</v>
       </c>
@@ -6100,12 +6463,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>690</v>
       </c>
@@ -6113,7 +6476,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>692</v>
       </c>
@@ -6134,17 +6497,17 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>250</v>
       </c>
@@ -6164,7 +6527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>729</v>
       </c>
@@ -6181,7 +6544,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D3" s="5" t="s">
         <v>731</v>
       </c>
@@ -6192,7 +6555,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D4" s="5" t="s">
         <v>732</v>
       </c>
@@ -6203,7 +6566,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" s="5" t="s">
         <v>733</v>
       </c>
@@ -6214,7 +6577,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D6" s="5" t="s">
         <v>734</v>
       </c>
@@ -6225,7 +6588,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>736</v>
       </c>
@@ -6239,7 +6602,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D8" s="5" t="s">
         <v>738</v>
       </c>
@@ -6250,7 +6613,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>709</v>
       </c>
@@ -6270,7 +6633,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" s="5" t="s">
         <v>748</v>
       </c>
@@ -6281,7 +6644,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" s="5" t="s">
         <v>749</v>
       </c>
@@ -6292,7 +6655,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="5" t="s">
         <v>521</v>
       </c>
@@ -6303,7 +6666,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" s="5" t="s">
         <v>750</v>
       </c>
@@ -6314,7 +6677,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" s="5" t="s">
         <v>751</v>
       </c>
@@ -6325,7 +6688,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" s="5" t="s">
         <v>752</v>
       </c>
@@ -6336,7 +6699,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" s="5" t="s">
         <v>753</v>
       </c>
@@ -6347,7 +6710,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D17" s="5" t="s">
         <v>754</v>
       </c>
@@ -6358,7 +6721,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D18" s="5" t="s">
         <v>755</v>
       </c>
@@ -6369,7 +6732,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>768</v>
       </c>
@@ -6383,7 +6746,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>771</v>
       </c>
@@ -6400,7 +6763,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D21" s="5" t="s">
         <v>731</v>
       </c>
@@ -6411,7 +6774,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D22" s="5" t="s">
         <v>732</v>
       </c>
@@ -6422,7 +6785,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>776</v>
       </c>
@@ -6439,7 +6802,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D24" s="5" t="s">
         <v>779</v>
       </c>
@@ -6450,7 +6813,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D25" s="5" t="s">
         <v>780</v>
       </c>
@@ -6461,7 +6824,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D26" s="5" t="s">
         <v>778</v>
       </c>
@@ -6472,7 +6835,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D27" s="5" t="s">
         <v>781</v>
       </c>
@@ -6483,7 +6846,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D28" s="5" t="s">
         <v>782</v>
       </c>
@@ -6494,7 +6857,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D29" s="5" t="s">
         <v>783</v>
       </c>
@@ -6505,7 +6868,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D30" s="5" t="s">
         <v>784</v>
       </c>
@@ -6516,7 +6879,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D31" s="5" t="s">
         <v>785</v>
       </c>
@@ -6540,22 +6903,22 @@
       <selection sqref="A1:J53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -6587,7 +6950,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -6619,7 +6982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -6651,7 +7014,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -6683,7 +7046,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -6715,7 +7078,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -6747,7 +7110,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -6779,7 +7142,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -6811,7 +7174,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -6843,7 +7206,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
@@ -6875,7 +7238,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>37</v>
       </c>
@@ -6907,7 +7270,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>39</v>
       </c>
@@ -6939,7 +7302,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>41</v>
       </c>
@@ -6971,7 +7334,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
@@ -7003,7 +7366,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
@@ -7035,7 +7398,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>54</v>
       </c>
@@ -7067,7 +7430,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>55</v>
       </c>
@@ -7099,7 +7462,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>56</v>
       </c>
@@ -7131,7 +7494,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>170</v>
       </c>
@@ -7160,7 +7523,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>171</v>
       </c>
@@ -7189,7 +7552,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>172</v>
       </c>
@@ -7218,7 +7581,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>173</v>
       </c>
@@ -7247,7 +7610,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>174</v>
       </c>
@@ -7276,7 +7639,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>73</v>
       </c>
@@ -7302,7 +7665,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>74</v>
       </c>
@@ -7328,7 +7691,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>75</v>
       </c>
@@ -7354,7 +7717,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
@@ -7380,7 +7743,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>77</v>
       </c>
@@ -7406,7 +7769,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>80</v>
       </c>
@@ -7432,7 +7795,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>81</v>
       </c>
@@ -7458,7 +7821,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>83</v>
       </c>
@@ -7484,7 +7847,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>84</v>
       </c>
@@ -7510,7 +7873,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>85</v>
       </c>
@@ -7536,7 +7899,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>94</v>
       </c>
@@ -7562,7 +7925,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>95</v>
       </c>
@@ -7588,7 +7951,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>96</v>
       </c>
@@ -7614,7 +7977,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>97</v>
       </c>
@@ -7640,7 +8003,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>98</v>
       </c>
@@ -7666,7 +8029,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>104</v>
       </c>
@@ -7692,7 +8055,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>105</v>
       </c>
@@ -7718,7 +8081,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>106</v>
       </c>
@@ -7744,7 +8107,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>107</v>
       </c>
@@ -7770,7 +8133,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>108</v>
       </c>
@@ -7796,7 +8159,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>113</v>
       </c>
@@ -7822,7 +8185,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>115</v>
       </c>
@@ -7848,7 +8211,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>116</v>
       </c>
@@ -7874,7 +8237,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>117</v>
       </c>
@@ -7900,7 +8263,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>118</v>
       </c>
@@ -7926,7 +8289,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>119</v>
       </c>
@@ -7952,7 +8315,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>120</v>
       </c>
@@ -7978,7 +8341,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>121</v>
       </c>
@@ -8004,7 +8367,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>122</v>
       </c>
@@ -8030,7 +8393,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>123</v>
       </c>
@@ -8069,20 +8432,20 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -8111,8 +8474,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
         <v>466</v>
       </c>
       <c r="C2" t="s">
@@ -8125,8 +8488,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
       <c r="C3" t="s">
         <v>698</v>
       </c>
@@ -8137,8 +8500,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
         <v>706</v>
       </c>
       <c r="C4" t="s">
@@ -8151,8 +8514,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="19"/>
       <c r="C5" t="s">
         <v>705</v>
       </c>
@@ -8163,7 +8526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>707</v>
       </c>
@@ -8194,21 +8557,21 @@
       <selection activeCell="A2" sqref="A2:I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -8237,7 +8600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>247</v>
       </c>
@@ -8257,7 +8620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>239</v>
       </c>
@@ -8277,7 +8640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>240</v>
       </c>
@@ -8297,7 +8660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>241</v>
       </c>
@@ -8317,7 +8680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>242</v>
       </c>
@@ -8337,7 +8700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>243</v>
       </c>
@@ -8360,7 +8723,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>244</v>
       </c>
@@ -8383,7 +8746,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>124</v>
       </c>
@@ -8403,7 +8766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>125</v>
       </c>
@@ -8423,7 +8786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>126</v>
       </c>
@@ -8443,7 +8806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>127</v>
       </c>
@@ -8463,7 +8826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>128</v>
       </c>
@@ -8483,7 +8846,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>694</v>
       </c>
@@ -8497,7 +8860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>695</v>
       </c>
@@ -8514,7 +8877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>696</v>
       </c>
@@ -8531,8 +8894,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
         <v>704</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -8548,8 +8911,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
       <c r="C18" s="1" t="s">
         <v>708</v>
       </c>
@@ -8580,16 +8943,16 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>249</v>
       </c>
@@ -8609,7 +8972,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>248</v>
       </c>
@@ -8629,7 +8992,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>257</v>
       </c>
@@ -8646,7 +9009,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>258</v>
       </c>
@@ -8663,7 +9026,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>259</v>
       </c>
@@ -8680,7 +9043,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>260</v>
       </c>
@@ -8697,7 +9060,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>261</v>
       </c>
@@ -8714,7 +9077,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>262</v>
       </c>
@@ -8731,7 +9094,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>263</v>
       </c>
@@ -8748,7 +9111,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>264</v>
       </c>
@@ -8765,7 +9128,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>265</v>
       </c>
@@ -8782,7 +9145,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>283</v>
       </c>
@@ -8799,7 +9162,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>266</v>
       </c>
@@ -8819,7 +9182,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>302</v>
       </c>
@@ -8836,7 +9199,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>303</v>
       </c>
@@ -8853,7 +9216,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>304</v>
       </c>
@@ -8870,7 +9233,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>290</v>
       </c>
@@ -8887,7 +9250,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>293</v>
       </c>
@@ -8904,7 +9267,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>295</v>
       </c>
@@ -8921,7 +9284,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>297</v>
       </c>
@@ -8938,7 +9301,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>299</v>
       </c>
@@ -8955,7 +9318,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>305</v>
       </c>
@@ -8972,7 +9335,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>307</v>
       </c>
@@ -8989,7 +9352,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>398</v>
       </c>
@@ -9006,7 +9369,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>401</v>
       </c>
@@ -9023,7 +9386,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>428</v>
       </c>
@@ -9037,7 +9400,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>429</v>
       </c>
@@ -9051,7 +9414,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>430</v>
       </c>
@@ -9065,7 +9428,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>431</v>
       </c>
@@ -9079,7 +9442,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>432</v>
       </c>
@@ -9093,7 +9456,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>433</v>
       </c>
@@ -9107,7 +9470,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>408</v>
       </c>
@@ -9121,7 +9484,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>312</v>
       </c>
@@ -9141,7 +9504,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>316</v>
       </c>
@@ -9158,7 +9521,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>318</v>
       </c>
@@ -9175,7 +9538,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>317</v>
       </c>
@@ -9189,7 +9552,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>321</v>
       </c>
@@ -9206,7 +9569,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>322</v>
       </c>
@@ -9223,7 +9586,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>323</v>
       </c>
@@ -9240,7 +9603,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>324</v>
       </c>
@@ -9254,7 +9617,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>325</v>
       </c>
@@ -9271,7 +9634,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>326</v>
       </c>
@@ -9288,7 +9651,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>327</v>
       </c>
@@ -9305,7 +9668,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>328</v>
       </c>
@@ -9319,7 +9682,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>329</v>
       </c>
@@ -9336,7 +9699,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>330</v>
       </c>
@@ -9353,7 +9716,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>331</v>
       </c>
@@ -9370,7 +9733,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>332</v>
       </c>
@@ -9384,7 +9747,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>333</v>
       </c>
@@ -9401,7 +9764,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>334</v>
       </c>
@@ -9418,7 +9781,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>335</v>
       </c>
@@ -9435,7 +9798,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>336</v>
       </c>
@@ -9449,7 +9812,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>358</v>
       </c>
@@ -9463,7 +9826,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>360</v>
       </c>
@@ -9477,7 +9840,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>363</v>
       </c>
@@ -9491,7 +9854,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>365</v>
       </c>
@@ -9505,7 +9868,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>367</v>
       </c>
@@ -9519,7 +9882,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>369</v>
       </c>
@@ -9533,7 +9896,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="59" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>372</v>
       </c>
@@ -9550,7 +9913,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>376</v>
       </c>
@@ -9567,7 +9930,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="61" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>379</v>
       </c>
@@ -9584,7 +9947,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>382</v>
       </c>
@@ -9601,7 +9964,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="63" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>385</v>
       </c>
@@ -9618,7 +9981,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="64" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>388</v>
       </c>
@@ -9632,7 +9995,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>390</v>
       </c>
@@ -9646,7 +10009,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>392</v>
       </c>
@@ -9660,7 +10023,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>394</v>
       </c>
@@ -9674,7 +10037,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>396</v>
       </c>
@@ -9688,7 +10051,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>402</v>
       </c>
@@ -9705,7 +10068,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>406</v>
       </c>
@@ -9719,7 +10082,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>411</v>
       </c>
@@ -9736,7 +10099,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>415</v>
       </c>
@@ -9750,7 +10113,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>418</v>
       </c>
@@ -9761,7 +10124,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>420</v>
       </c>
@@ -9775,7 +10138,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>423</v>
       </c>
@@ -9789,7 +10152,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>425</v>
       </c>
@@ -9814,15 +10177,15 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>441</v>
       </c>
@@ -9836,7 +10199,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>402</v>
       </c>
@@ -9850,7 +10213,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>446</v>
       </c>
@@ -9861,7 +10224,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>449</v>
       </c>
@@ -9872,7 +10235,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>452</v>
       </c>
@@ -9883,7 +10246,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>454</v>
       </c>
@@ -9894,7 +10257,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>457</v>
       </c>
@@ -9905,7 +10268,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>459</v>
       </c>
@@ -9916,7 +10279,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>461</v>
       </c>
@@ -9927,7 +10290,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>463</v>
       </c>
@@ -9941,7 +10304,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>466</v>
       </c>
@@ -9955,7 +10318,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>469</v>
       </c>
@@ -9966,7 +10329,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>471</v>
       </c>
@@ -9977,7 +10340,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>473</v>
       </c>
@@ -9988,7 +10351,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>266</v>
       </c>
@@ -10002,7 +10365,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>477</v>
       </c>
@@ -10013,7 +10376,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>479</v>
       </c>
@@ -10024,7 +10387,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>481</v>
       </c>
@@ -10035,7 +10398,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>483</v>
       </c>
@@ -10046,7 +10409,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>485</v>
       </c>
@@ -10057,7 +10420,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>487</v>
       </c>
@@ -10068,7 +10431,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>490</v>
       </c>
@@ -10079,7 +10442,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>312</v>
       </c>
@@ -10093,7 +10456,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>494</v>
       </c>
@@ -10104,7 +10467,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>496</v>
       </c>
@@ -10115,7 +10478,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>498</v>
       </c>
@@ -10126,7 +10489,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>500</v>
       </c>
@@ -10137,7 +10500,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>503</v>
       </c>
@@ -10148,7 +10511,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>505</v>
       </c>
@@ -10159,7 +10522,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>507</v>
       </c>
@@ -10170,7 +10533,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>509</v>
       </c>
@@ -10181,7 +10544,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>511</v>
       </c>
@@ -10192,7 +10555,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>512</v>
       </c>
@@ -10203,7 +10566,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>515</v>
       </c>
@@ -10217,7 +10580,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>519</v>
       </c>
@@ -10228,7 +10591,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>520</v>
       </c>
@@ -10239,7 +10602,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>521</v>
       </c>
@@ -10250,7 +10613,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>525</v>
       </c>
@@ -10264,7 +10627,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>528</v>
       </c>
@@ -10289,20 +10652,20 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" style="6" customWidth="1"/>
     <col min="6" max="6" width="41" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41" style="6" customWidth="1"/>
     <col min="8" max="8" width="15" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="6"/>
+    <col min="9" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>531</v>
       </c>
@@ -10328,7 +10691,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>411</v>
       </c>
@@ -10357,7 +10720,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C3" s="6">
         <v>1</v>
       </c>
@@ -10380,7 +10743,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>540</v>
       </c>
@@ -10397,7 +10760,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>542</v>
       </c>
@@ -10411,7 +10774,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>418</v>
       </c>
@@ -10425,7 +10788,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>545</v>
       </c>
@@ -10451,7 +10814,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>556</v>
       </c>
@@ -10477,7 +10840,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C9" s="6">
         <v>3000</v>
       </c>
@@ -10497,7 +10860,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C10" s="6">
         <v>4000</v>
       </c>
@@ -10517,7 +10880,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C11" s="6">
         <v>500</v>
       </c>
@@ -10537,7 +10900,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>572</v>
       </c>
@@ -10551,7 +10914,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C13" s="6">
         <v>2000</v>
       </c>
@@ -10559,7 +10922,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C14" s="6">
         <v>4000</v>
       </c>
@@ -10567,7 +10930,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>573</v>
       </c>
@@ -10584,7 +10947,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C16" s="6" t="s">
         <v>575</v>
       </c>
@@ -10598,7 +10961,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>579</v>
       </c>
@@ -10606,7 +10969,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>580</v>
       </c>
@@ -10617,7 +10980,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C19" s="6" t="s">
         <v>584</v>
       </c>
@@ -10625,7 +10988,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C20" s="6" t="s">
         <v>586</v>
       </c>
@@ -10633,7 +10996,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C21" s="6" t="s">
         <v>588</v>
       </c>
@@ -10641,7 +11004,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C22" s="6" t="s">
         <v>590</v>
       </c>
@@ -10649,7 +11012,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C23" s="6" t="s">
         <v>592</v>
       </c>
@@ -10657,7 +11020,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C24" s="6" t="s">
         <v>594</v>
       </c>
@@ -10665,7 +11028,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C25" s="6" t="s">
         <v>596</v>
       </c>
@@ -10673,7 +11036,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C26" s="6" t="s">
         <v>598</v>
       </c>
@@ -10681,7 +11044,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C27" s="6" t="s">
         <v>600</v>
       </c>
@@ -10689,7 +11052,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
         <v>602</v>
       </c>
@@ -10700,7 +11063,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C29" s="6">
         <v>1</v>
       </c>
@@ -10722,17 +11085,17 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="9"/>
-    <col min="5" max="5" width="42.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="9"/>
+    <col min="5" max="5" width="42.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>531</v>
       </c>
@@ -10752,7 +11115,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>411</v>
       </c>
@@ -10769,7 +11132,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>418</v>
       </c>
@@ -10783,7 +11146,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>610</v>
       </c>
@@ -10800,7 +11163,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>530</v>
       </c>
@@ -10817,7 +11180,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>542</v>
       </c>
@@ -10831,7 +11194,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
         <v>545</v>
       </c>
@@ -10841,34 +11204,34 @@
       <c r="D7" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="20" t="s">
         <v>621</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="18" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" s="9" t="s">
         <v>617</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="20"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="20"/>
+      <c r="F8" s="18"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" s="9" t="s">
         <v>618</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="20"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E9" s="20"/>
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>540</v>
       </c>
@@ -10885,7 +11248,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>556</v>
       </c>
@@ -10905,7 +11268,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
         <v>572</v>
       </c>
@@ -10922,7 +11285,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
         <v>573</v>
       </c>
@@ -10939,7 +11302,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>629</v>
       </c>
@@ -10952,28 +11315,28 @@
       <c r="D14" s="9" t="s">
         <v>619</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="20" t="s">
         <v>632</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="18" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" s="9" t="s">
         <v>631</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>619</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="20"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E16" s="17"/>
-      <c r="F16" s="20"/>
-    </row>
-    <row r="17" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E15" s="20"/>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="20"/>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
         <v>633</v>
       </c>
@@ -10990,7 +11353,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
         <v>635</v>
       </c>
@@ -11004,7 +11367,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="9" t="s">
         <v>602</v>
       </c>
@@ -11018,7 +11381,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
         <v>639</v>
       </c>
@@ -11032,7 +11395,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
         <v>642</v>
       </c>
@@ -11046,7 +11409,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>645</v>
       </c>
@@ -11060,7 +11423,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
         <v>648</v>
       </c>
@@ -11074,7 +11437,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
         <v>651</v>
       </c>
@@ -11091,7 +11454,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="9" t="s">
         <v>580</v>
       </c>
@@ -11101,24 +11464,24 @@
       <c r="D25" s="9" t="s">
         <v>517</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="20" t="s">
         <v>654</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="18" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C26" s="9" t="s">
         <v>640</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>517</v>
       </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="20"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="20"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="9" t="s">
         <v>655</v>
       </c>
@@ -11128,32 +11491,32 @@
       <c r="D27" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="20" t="s">
         <v>657</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="18" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C28" s="9" t="s">
         <v>617</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="20"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="20"/>
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C29" s="9" t="s">
         <v>656</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
New version of the signals list with more DIO.
</commit_message>
<xml_diff>
--- a/Support/Signal List.xlsx
+++ b/Support/Signal List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9648" windowHeight="3876"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9645" windowHeight="3870"/>
   </bookViews>
   <sheets>
     <sheet name="DAQ Signals All" sheetId="11" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1688" uniqueCount="842">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="863">
   <si>
     <t>Speaker Out</t>
   </si>
@@ -3575,9 +3575,6 @@
     <t>Inlet LED</t>
   </si>
   <si>
-    <t>P2.0</t>
-  </si>
-  <si>
     <t>P2.1</t>
   </si>
   <si>
@@ -3666,6 +3663,72 @@
   </si>
   <si>
     <t>ctr0</t>
+  </si>
+  <si>
+    <t>O3 Generator Enable</t>
+  </si>
+  <si>
+    <t>Denuder Enable</t>
+  </si>
+  <si>
+    <t>Laser PS Enable</t>
+  </si>
+  <si>
+    <t>P0.7</t>
+  </si>
+  <si>
+    <t>TEC PS Enable</t>
+  </si>
+  <si>
+    <t>Sample Pump Block</t>
+  </si>
+  <si>
+    <t>Laser Interlock</t>
+  </si>
+  <si>
+    <t>P1.2</t>
+  </si>
+  <si>
+    <t>Blocked Impactor</t>
+  </si>
+  <si>
+    <t>P1.3</t>
+  </si>
+  <si>
+    <t>Signal from pressure differential sensor to indicate blocked impactor</t>
+  </si>
+  <si>
+    <t>Input from laser enclosure interlock</t>
+  </si>
+  <si>
+    <t>Input from sample pump indicating blockage</t>
+  </si>
+  <si>
+    <t>51,18</t>
+  </si>
+  <si>
+    <t>16,50</t>
+  </si>
+  <si>
+    <t>48,15</t>
+  </si>
+  <si>
+    <t>11,44</t>
+  </si>
+  <si>
+    <t>10,44</t>
+  </si>
+  <si>
+    <t>43,9</t>
+  </si>
+  <si>
+    <t>Output for PWM of ozone generator</t>
+  </si>
+  <si>
+    <t>41,7</t>
+  </si>
+  <si>
+    <t>P1.4</t>
   </si>
 </sst>
 </file>
@@ -3697,12 +3760,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3717,7 +3786,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3762,19 +3831,23 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4056,27 +4129,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="75.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="75.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>713</v>
       </c>
@@ -4108,7 +4181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>312</v>
       </c>
@@ -4140,7 +4213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
@@ -4169,7 +4242,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
@@ -4198,7 +4271,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
@@ -4227,7 +4300,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -4256,7 +4329,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
@@ -4285,7 +4358,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
@@ -4314,7 +4387,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
@@ -4343,7 +4416,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>35</v>
       </c>
@@ -4372,7 +4445,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>37</v>
       </c>
@@ -4401,7 +4474,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
@@ -4430,7 +4503,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>41</v>
       </c>
@@ -4459,7 +4532,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>51</v>
       </c>
@@ -4488,7 +4561,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>53</v>
       </c>
@@ -4517,7 +4590,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>54</v>
       </c>
@@ -4546,7 +4619,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>55</v>
       </c>
@@ -4575,7 +4648,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>56</v>
       </c>
@@ -4604,7 +4677,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>170</v>
       </c>
@@ -4631,7 +4704,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>171</v>
       </c>
@@ -4658,7 +4731,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>172</v>
       </c>
@@ -4685,7 +4758,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>173</v>
       </c>
@@ -4712,7 +4785,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>174</v>
       </c>
@@ -4739,7 +4812,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>73</v>
       </c>
@@ -4766,7 +4839,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>74</v>
       </c>
@@ -4793,7 +4866,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>75</v>
       </c>
@@ -4820,7 +4893,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>76</v>
       </c>
@@ -4847,7 +4920,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>77</v>
       </c>
@@ -4874,7 +4947,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>80</v>
       </c>
@@ -4901,7 +4974,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>81</v>
       </c>
@@ -4928,7 +5001,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>83</v>
       </c>
@@ -4955,7 +5028,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>84</v>
       </c>
@@ -4982,7 +5055,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>85</v>
       </c>
@@ -5009,7 +5082,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>94</v>
       </c>
@@ -5036,7 +5109,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>95</v>
       </c>
@@ -5063,7 +5136,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>96</v>
       </c>
@@ -5090,7 +5163,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>97</v>
       </c>
@@ -5117,7 +5190,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>98</v>
       </c>
@@ -5144,7 +5217,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>104</v>
       </c>
@@ -5171,7 +5244,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
         <v>105</v>
       </c>
@@ -5198,7 +5271,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
         <v>106</v>
       </c>
@@ -5225,7 +5298,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>107</v>
       </c>
@@ -5252,7 +5325,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>108</v>
       </c>
@@ -5279,8 +5352,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B44" s="17" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="20" t="s">
         <v>704</v>
       </c>
       <c r="C44" s="1"/>
@@ -5293,43 +5366,43 @@
       <c r="F44" s="1">
         <v>0</v>
       </c>
-      <c r="G44" s="18">
+      <c r="G44" s="17">
         <v>6225</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="17" t="s">
         <v>114</v>
       </c>
       <c r="I44" s="1">
         <v>6</v>
       </c>
-      <c r="J44" s="21" t="s">
+      <c r="J44" s="19" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B45" s="17"/>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="20"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
         <v>698</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="F45" s="1">
         <v>0</v>
       </c>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
       <c r="I45" s="1">
         <v>6</v>
       </c>
-      <c r="J45" s="21"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J45" s="19"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>411</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="21" t="s">
         <v>797</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -5339,36 +5412,36 @@
       <c r="F46" s="1">
         <v>0</v>
       </c>
-      <c r="G46" s="18">
+      <c r="G46" s="17">
         <v>6225</v>
       </c>
-      <c r="H46" s="18" t="s">
+      <c r="H46" s="17" t="s">
         <v>114</v>
       </c>
       <c r="I46" s="1">
         <v>7</v>
       </c>
-      <c r="J46" s="20" t="s">
+      <c r="J46" s="18" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B47" s="19"/>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="21"/>
       <c r="D47" s="1" t="s">
         <v>698</v>
       </c>
       <c r="F47" s="1">
         <v>0</v>
       </c>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
       <c r="I47" s="1">
         <v>7</v>
       </c>
-      <c r="J47" s="20"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B48" s="19" t="s">
+      <c r="J47" s="18"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="21" t="s">
         <v>799</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -5382,12 +5455,12 @@
       <c r="I48" s="1">
         <v>7</v>
       </c>
-      <c r="J48" s="20" t="s">
+      <c r="J48" s="18" t="s">
         <v>803</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B49" s="19"/>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" s="21"/>
       <c r="D49" s="1" t="s">
         <v>801</v>
       </c>
@@ -5399,10 +5472,10 @@
       <c r="I49" s="1">
         <v>7</v>
       </c>
-      <c r="J49" s="20"/>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B50" s="19" t="s">
+      <c r="J49" s="18"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="21" t="s">
         <v>798</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -5411,36 +5484,36 @@
       <c r="F50" s="1">
         <v>0</v>
       </c>
-      <c r="G50" s="18">
+      <c r="G50" s="17">
         <v>6225</v>
       </c>
-      <c r="H50" s="18" t="s">
+      <c r="H50" s="17" t="s">
         <v>114</v>
       </c>
       <c r="I50" s="1">
         <v>7</v>
       </c>
-      <c r="J50" s="20" t="s">
+      <c r="J50" s="18" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B51" s="19"/>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="21"/>
       <c r="D51" s="1" t="s">
         <v>705</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
       </c>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
       <c r="I51" s="1">
         <v>7</v>
       </c>
-      <c r="J51" s="20"/>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B52" s="19" t="s">
+      <c r="J51" s="18"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="21" t="s">
         <v>802</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -5454,12 +5527,12 @@
       <c r="I52" s="1">
         <v>7</v>
       </c>
-      <c r="J52" s="20" t="s">
+      <c r="J52" s="18" t="s">
         <v>804</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B53" s="19"/>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="21"/>
       <c r="D53" s="1" t="s">
         <v>806</v>
       </c>
@@ -5471,9 +5544,9 @@
       <c r="I53" s="1">
         <v>7</v>
       </c>
-      <c r="J53" s="20"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J53" s="18"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>707</v>
       </c>
@@ -5496,15 +5569,15 @@
         <v>794</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>810</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>811</v>
+        <v>862</v>
       </c>
       <c r="E55" t="s">
-        <v>831</v>
+        <v>861</v>
       </c>
       <c r="F55" s="1">
         <v>0</v>
@@ -5519,15 +5592,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E56" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="F56" s="1">
         <v>0</v>
@@ -5542,15 +5615,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E57" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F57" s="1">
         <v>0</v>
@@ -5565,15 +5638,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E58" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="F58" s="1">
         <v>0</v>
@@ -5588,15 +5661,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E59" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="F59" s="1">
         <v>0</v>
@@ -5611,12 +5684,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E60" t="s">
         <v>233</v>
@@ -5634,15 +5707,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E61" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="F61" s="1">
         <v>0</v>
@@ -5657,15 +5730,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E62" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="F62" s="1">
         <v>0</v>
@@ -5680,15 +5753,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>703</v>
       </c>
       <c r="E63" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F63" s="1">
         <v>0</v>
@@ -5703,15 +5776,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>705</v>
       </c>
       <c r="E64" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="F64" s="1">
         <v>0</v>
@@ -5726,15 +5799,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>708</v>
       </c>
       <c r="E65" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="F65" s="1">
         <v>0</v>
@@ -5749,147 +5822,159 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>841</v>
-      </c>
-      <c r="H66" s="1"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>266</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>719</v>
-      </c>
-      <c r="C67" s="1"/>
+        <v>800</v>
+      </c>
+      <c r="E66" t="s">
+        <v>854</v>
+      </c>
+      <c r="F66" s="1">
+        <v>0</v>
+      </c>
+      <c r="G66" s="1">
+        <v>6225</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I66" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>842</v>
+      </c>
       <c r="D67" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>175</v>
+        <v>801</v>
+      </c>
+      <c r="E67" t="s">
+        <v>855</v>
       </c>
       <c r="F67" s="1">
         <v>0</v>
       </c>
       <c r="G67" s="1">
-        <v>6124</v>
-      </c>
-      <c r="H67" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I67" s="1">
-        <v>3</v>
-      </c>
-      <c r="J67" s="3" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B68" s="17"/>
-      <c r="C68" s="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>843</v>
+      </c>
       <c r="D68" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>231</v>
+        <v>844</v>
+      </c>
+      <c r="E68" t="s">
+        <v>856</v>
       </c>
       <c r="F68" s="1">
         <v>0</v>
       </c>
       <c r="G68" s="1">
-        <v>6124</v>
-      </c>
-      <c r="H68" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I68" s="1">
-        <v>3</v>
-      </c>
-      <c r="J68" s="3" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B69" s="17"/>
-      <c r="C69" s="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>845</v>
+      </c>
       <c r="D69" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>177</v>
+        <v>805</v>
+      </c>
+      <c r="E69" t="s">
+        <v>857</v>
       </c>
       <c r="F69" s="1">
         <v>0</v>
       </c>
       <c r="G69" s="1">
-        <v>6124</v>
-      </c>
-      <c r="H69" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I69" s="1">
-        <v>3</v>
-      </c>
-      <c r="J69" s="3" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B70" s="17"/>
-      <c r="C70" s="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>846</v>
+      </c>
       <c r="D70" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>232</v>
+        <v>806</v>
+      </c>
+      <c r="E70" t="s">
+        <v>858</v>
       </c>
       <c r="F70" s="1">
         <v>0</v>
       </c>
       <c r="G70" s="1">
-        <v>6124</v>
-      </c>
-      <c r="H70" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I70" s="1">
-        <v>3</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B71" s="3" t="s">
-        <v>720</v>
-      </c>
-      <c r="C71" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="J70" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>847</v>
+      </c>
       <c r="D71" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>175</v>
+        <v>848</v>
+      </c>
+      <c r="E71" t="s">
+        <v>859</v>
       </c>
       <c r="F71" s="1">
         <v>0</v>
       </c>
       <c r="G71" s="1">
-        <v>6132</v>
-      </c>
-      <c r="H71" s="1"/>
+        <v>6225</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I71" s="1">
-        <v>5</v>
-      </c>
-      <c r="J71" s="3" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B72" s="3" t="s">
-        <v>721</v>
-      </c>
-      <c r="C72" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="J71" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>849</v>
+      </c>
       <c r="D72" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>160</v>
+        <v>850</v>
+      </c>
+      <c r="E72" t="s">
+        <v>58</v>
       </c>
       <c r="F72" s="1">
         <v>0</v>
@@ -5897,155 +5982,178 @@
       <c r="G72" s="1">
         <v>6225</v>
       </c>
-      <c r="H72" s="1"/>
+      <c r="H72" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="I72" s="1">
-        <v>8</v>
-      </c>
-      <c r="J72" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B73" s="3" t="s">
-        <v>722</v>
-      </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="F73" s="1">
+        <v>6</v>
+      </c>
+      <c r="J72" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="22" t="s">
+        <v>839</v>
+      </c>
+      <c r="D73" s="23" t="s">
+        <v>840</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>830</v>
+      </c>
+      <c r="F73" s="23">
         <v>0</v>
       </c>
-      <c r="G73" s="1">
+      <c r="G73" s="23">
         <v>6225</v>
       </c>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1">
-        <v>8</v>
-      </c>
-      <c r="J73" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B74" s="17" t="s">
-        <v>723</v>
+      <c r="H73" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="I73" s="23">
+        <v>6</v>
+      </c>
+      <c r="J73" s="22" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>266</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>719</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>111</v>
+        <v>175</v>
+      </c>
+      <c r="F74" s="1">
+        <v>0</v>
       </c>
       <c r="G74" s="1">
-        <v>6704</v>
+        <v>6124</v>
       </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1">
-        <v>6</v>
-      </c>
-      <c r="J74" s="3"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B75" s="17"/>
+        <v>3</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B75" s="20"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>699</v>
+        <v>67</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>111</v>
+        <v>231</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0</v>
       </c>
       <c r="G75" s="1">
-        <v>6704</v>
+        <v>6124</v>
       </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1">
-        <v>6</v>
-      </c>
-      <c r="J75" s="3"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B76" s="17"/>
+        <v>3</v>
+      </c>
+      <c r="J75" s="3" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B76" s="20"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>700</v>
+        <v>68</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>111</v>
+        <v>177</v>
+      </c>
+      <c r="F76" s="1">
+        <v>0</v>
       </c>
       <c r="G76" s="1">
-        <v>6704</v>
+        <v>6124</v>
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1">
-        <v>6</v>
-      </c>
-      <c r="J76" s="3"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B77" s="17"/>
+        <v>3</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B77" s="20"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
-        <v>701</v>
+        <v>69</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>111</v>
+        <v>232</v>
+      </c>
+      <c r="F77" s="1">
+        <v>0</v>
       </c>
       <c r="G77" s="1">
-        <v>6704</v>
+        <v>6124</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1">
-        <v>6</v>
-      </c>
-      <c r="J77" s="3"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B78" s="17"/>
+        <v>3</v>
+      </c>
+      <c r="J77" s="3" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B78" s="3" t="s">
+        <v>720</v>
+      </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>702</v>
+        <v>66</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>111</v>
+        <v>175</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0</v>
       </c>
       <c r="G78" s="1">
-        <v>6704</v>
+        <v>6132</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1">
-        <v>6</v>
-      </c>
-      <c r="J78" s="3"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="J78" s="3" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="E79" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F79" s="1">
+        <v>0</v>
+      </c>
       <c r="G79" s="1">
         <v>6225</v>
       </c>
@@ -6054,18 +6162,20 @@
         <v>8</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B80" s="17" t="s">
-        <v>725</v>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B80" s="3" t="s">
+        <v>722</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>698</v>
-      </c>
-      <c r="E80" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="F80" s="1">
         <v>0</v>
       </c>
@@ -6077,68 +6187,229 @@
         <v>8</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B81" s="17"/>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B81" s="20" t="s">
+        <v>723</v>
+      </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>703</v>
-      </c>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="G81" s="1">
-        <v>6225</v>
+        <v>6704</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1">
-        <v>8</v>
-      </c>
-      <c r="J81" s="3" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B82" s="16" t="s">
-        <v>807</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="J81" s="3"/>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B82" s="20"/>
+      <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>5</v>
+        <v>699</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="G82" s="1">
         <v>6704</v>
       </c>
-    </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B83" s="16" t="s">
-        <v>808</v>
-      </c>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1">
+        <v>6</v>
+      </c>
+      <c r="J82" s="3"/>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B83" s="20"/>
+      <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>14</v>
+        <v>700</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="G83" s="1">
         <v>6704</v>
       </c>
-    </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B84" s="3" t="s">
-        <v>809</v>
-      </c>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1">
+        <v>6</v>
+      </c>
+      <c r="J83" s="3"/>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B84" s="20"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E84" s="1"/>
+        <v>701</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="G84" s="1">
         <v>6704</v>
       </c>
       <c r="H84" s="1"/>
+      <c r="I84" s="1">
+        <v>6</v>
+      </c>
+      <c r="J84" s="3"/>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B85" s="20"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G85" s="1">
+        <v>6704</v>
+      </c>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1">
+        <v>6</v>
+      </c>
+      <c r="J85" s="3"/>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B86" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="E86" s="1"/>
+      <c r="G86" s="1">
+        <v>6225</v>
+      </c>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1">
+        <v>7</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B87" s="20" t="s">
+        <v>725</v>
+      </c>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1">
+        <v>0</v>
+      </c>
+      <c r="G87" s="1">
+        <v>6225</v>
+      </c>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1">
+        <v>7</v>
+      </c>
+      <c r="J87" s="3" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B88" s="20"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1">
+        <v>0</v>
+      </c>
+      <c r="G88" s="1">
+        <v>6225</v>
+      </c>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1">
+        <v>7</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B89" s="16" t="s">
+        <v>807</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G89" s="1">
+        <v>6704</v>
+      </c>
+    </row>
+    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B90" s="16" t="s">
+        <v>808</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G90" s="1">
+        <v>6704</v>
+      </c>
+    </row>
+    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B91" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E91" s="1"/>
+      <c r="G91" s="1">
+        <v>6704</v>
+      </c>
+      <c r="H91" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="B81:B85"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B52:B53"/>
     <mergeCell ref="H44:H45"/>
     <mergeCell ref="H46:H47"/>
     <mergeCell ref="H50:H51"/>
@@ -6147,17 +6418,6 @@
     <mergeCell ref="J50:J51"/>
     <mergeCell ref="J44:J45"/>
     <mergeCell ref="J46:J47"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="B74:B78"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B52:B53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6172,12 +6432,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>312</v>
       </c>
@@ -6188,7 +6448,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>660</v>
       </c>
@@ -6196,7 +6456,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>509</v>
       </c>
@@ -6204,7 +6464,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>511</v>
       </c>
@@ -6212,7 +6472,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>512</v>
       </c>
@@ -6220,7 +6480,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>661</v>
       </c>
@@ -6228,7 +6488,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>662</v>
       </c>
@@ -6236,7 +6496,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>663</v>
       </c>
@@ -6244,7 +6504,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>664</v>
       </c>
@@ -6252,7 +6512,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>665</v>
       </c>
@@ -6260,7 +6520,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>666</v>
       </c>
@@ -6268,7 +6528,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>667</v>
       </c>
@@ -6276,7 +6536,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>668</v>
       </c>
@@ -6284,7 +6544,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>669</v>
       </c>
@@ -6292,7 +6552,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>670</v>
       </c>
@@ -6300,7 +6560,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>671</v>
       </c>
@@ -6308,7 +6568,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>266</v>
       </c>
@@ -6319,7 +6579,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>572</v>
       </c>
@@ -6327,7 +6587,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>672</v>
       </c>
@@ -6335,7 +6595,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>411</v>
       </c>
@@ -6346,7 +6606,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>674</v>
       </c>
@@ -6354,7 +6614,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>675</v>
       </c>
@@ -6362,7 +6622,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>676</v>
       </c>
@@ -6370,7 +6630,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>684</v>
       </c>
@@ -6378,7 +6638,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>677</v>
       </c>
@@ -6386,7 +6646,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>515</v>
       </c>
@@ -6394,22 +6654,22 @@
         <v>679</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>402</v>
       </c>
@@ -6417,17 +6677,17 @@
         <v>680</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>683</v>
       </c>
@@ -6435,17 +6695,17 @@
         <v>483</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>521</v>
       </c>
@@ -6463,12 +6723,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>690</v>
       </c>
@@ -6476,7 +6736,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>692</v>
       </c>
@@ -6497,17 +6757,17 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>250</v>
       </c>
@@ -6527,7 +6787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>729</v>
       </c>
@@ -6544,7 +6804,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
         <v>731</v>
       </c>
@@ -6555,7 +6815,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="5" t="s">
         <v>732</v>
       </c>
@@ -6566,7 +6826,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" s="5" t="s">
         <v>733</v>
       </c>
@@ -6577,7 +6837,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="5" t="s">
         <v>734</v>
       </c>
@@ -6588,7 +6848,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>736</v>
       </c>
@@ -6602,7 +6862,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" s="5" t="s">
         <v>738</v>
       </c>
@@ -6613,7 +6873,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>709</v>
       </c>
@@ -6633,7 +6893,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" s="5" t="s">
         <v>748</v>
       </c>
@@ -6644,7 +6904,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" s="5" t="s">
         <v>749</v>
       </c>
@@ -6655,7 +6915,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
         <v>521</v>
       </c>
@@ -6666,7 +6926,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13" s="5" t="s">
         <v>750</v>
       </c>
@@ -6677,7 +6937,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
         <v>751</v>
       </c>
@@ -6688,7 +6948,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" s="5" t="s">
         <v>752</v>
       </c>
@@ -6699,7 +6959,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" s="5" t="s">
         <v>753</v>
       </c>
@@ -6710,7 +6970,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D17" s="5" t="s">
         <v>754</v>
       </c>
@@ -6721,7 +6981,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D18" s="5" t="s">
         <v>755</v>
       </c>
@@ -6732,7 +6992,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>768</v>
       </c>
@@ -6746,7 +7006,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>771</v>
       </c>
@@ -6763,7 +7023,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D21" s="5" t="s">
         <v>731</v>
       </c>
@@ -6774,7 +7034,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D22" s="5" t="s">
         <v>732</v>
       </c>
@@ -6785,7 +7045,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>776</v>
       </c>
@@ -6802,7 +7062,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" s="5" t="s">
         <v>779</v>
       </c>
@@ -6813,7 +7073,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D25" s="5" t="s">
         <v>780</v>
       </c>
@@ -6824,7 +7084,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D26" s="5" t="s">
         <v>778</v>
       </c>
@@ -6835,7 +7095,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D27" s="5" t="s">
         <v>781</v>
       </c>
@@ -6846,7 +7106,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D28" s="5" t="s">
         <v>782</v>
       </c>
@@ -6857,7 +7117,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D29" s="5" t="s">
         <v>783</v>
       </c>
@@ -6868,7 +7128,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D30" s="5" t="s">
         <v>784</v>
       </c>
@@ -6879,7 +7139,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D31" s="5" t="s">
         <v>785</v>
       </c>
@@ -6903,22 +7163,22 @@
       <selection sqref="A1:J53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -6950,7 +7210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -6982,7 +7242,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -7014,7 +7274,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -7046,7 +7306,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -7078,7 +7338,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -7110,7 +7370,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -7142,7 +7402,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -7174,7 +7434,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -7206,7 +7466,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
@@ -7238,7 +7498,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>37</v>
       </c>
@@ -7270,7 +7530,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>39</v>
       </c>
@@ -7302,7 +7562,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>41</v>
       </c>
@@ -7334,7 +7594,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
@@ -7366,7 +7626,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
@@ -7398,7 +7658,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>54</v>
       </c>
@@ -7430,7 +7690,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>55</v>
       </c>
@@ -7462,7 +7722,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>56</v>
       </c>
@@ -7494,7 +7754,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>170</v>
       </c>
@@ -7523,7 +7783,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>171</v>
       </c>
@@ -7552,7 +7812,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>172</v>
       </c>
@@ -7581,7 +7841,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>173</v>
       </c>
@@ -7610,7 +7870,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>174</v>
       </c>
@@ -7639,7 +7899,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>73</v>
       </c>
@@ -7665,7 +7925,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>74</v>
       </c>
@@ -7691,7 +7951,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>75</v>
       </c>
@@ -7717,7 +7977,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
@@ -7743,7 +8003,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>77</v>
       </c>
@@ -7769,7 +8029,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>80</v>
       </c>
@@ -7795,7 +8055,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>81</v>
       </c>
@@ -7821,7 +8081,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>83</v>
       </c>
@@ -7847,7 +8107,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>84</v>
       </c>
@@ -7873,7 +8133,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>85</v>
       </c>
@@ -7899,7 +8159,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>94</v>
       </c>
@@ -7925,7 +8185,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>95</v>
       </c>
@@ -7951,7 +8211,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>96</v>
       </c>
@@ -7977,7 +8237,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>97</v>
       </c>
@@ -8003,7 +8263,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>98</v>
       </c>
@@ -8029,7 +8289,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>104</v>
       </c>
@@ -8055,7 +8315,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>105</v>
       </c>
@@ -8081,7 +8341,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>106</v>
       </c>
@@ -8107,7 +8367,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>107</v>
       </c>
@@ -8133,7 +8393,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>108</v>
       </c>
@@ -8159,7 +8419,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>113</v>
       </c>
@@ -8185,7 +8445,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>115</v>
       </c>
@@ -8211,7 +8471,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>116</v>
       </c>
@@ -8237,7 +8497,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>117</v>
       </c>
@@ -8263,7 +8523,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>118</v>
       </c>
@@ -8289,7 +8549,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>119</v>
       </c>
@@ -8315,7 +8575,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>120</v>
       </c>
@@ -8341,7 +8601,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>121</v>
       </c>
@@ -8367,7 +8627,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>122</v>
       </c>
@@ -8393,7 +8653,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>123</v>
       </c>
@@ -8432,20 +8692,20 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -8474,8 +8734,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>466</v>
       </c>
       <c r="C2" t="s">
@@ -8488,8 +8748,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
       <c r="C3" t="s">
         <v>698</v>
       </c>
@@ -8500,8 +8760,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>706</v>
       </c>
       <c r="C4" t="s">
@@ -8514,8 +8774,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="21"/>
       <c r="C5" t="s">
         <v>705</v>
       </c>
@@ -8526,7 +8786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>707</v>
       </c>
@@ -8557,21 +8817,21 @@
       <selection activeCell="A2" sqref="A2:I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -8600,7 +8860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>247</v>
       </c>
@@ -8620,7 +8880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>239</v>
       </c>
@@ -8640,7 +8900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>240</v>
       </c>
@@ -8660,7 +8920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>241</v>
       </c>
@@ -8680,7 +8940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>242</v>
       </c>
@@ -8700,7 +8960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>243</v>
       </c>
@@ -8723,7 +8983,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>244</v>
       </c>
@@ -8746,7 +9006,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>124</v>
       </c>
@@ -8766,7 +9026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>125</v>
       </c>
@@ -8786,7 +9046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>126</v>
       </c>
@@ -8806,7 +9066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>127</v>
       </c>
@@ -8826,7 +9086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>128</v>
       </c>
@@ -8846,7 +9106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>694</v>
       </c>
@@ -8860,7 +9120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>695</v>
       </c>
@@ -8877,7 +9137,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>696</v>
       </c>
@@ -8894,8 +9154,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>704</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -8911,8 +9171,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
       <c r="C18" s="1" t="s">
         <v>708</v>
       </c>
@@ -8943,16 +9203,16 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>249</v>
       </c>
@@ -8972,7 +9232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>248</v>
       </c>
@@ -8992,7 +9252,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>257</v>
       </c>
@@ -9009,7 +9269,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>258</v>
       </c>
@@ -9026,7 +9286,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>259</v>
       </c>
@@ -9043,7 +9303,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>260</v>
       </c>
@@ -9060,7 +9320,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>261</v>
       </c>
@@ -9077,7 +9337,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>262</v>
       </c>
@@ -9094,7 +9354,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>263</v>
       </c>
@@ -9111,7 +9371,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>264</v>
       </c>
@@ -9128,7 +9388,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>265</v>
       </c>
@@ -9145,7 +9405,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>283</v>
       </c>
@@ -9162,7 +9422,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>266</v>
       </c>
@@ -9182,7 +9442,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>302</v>
       </c>
@@ -9199,7 +9459,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>303</v>
       </c>
@@ -9216,7 +9476,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>304</v>
       </c>
@@ -9233,7 +9493,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>290</v>
       </c>
@@ -9250,7 +9510,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>293</v>
       </c>
@@ -9267,7 +9527,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>295</v>
       </c>
@@ -9284,7 +9544,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>297</v>
       </c>
@@ -9301,7 +9561,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>299</v>
       </c>
@@ -9318,7 +9578,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>305</v>
       </c>
@@ -9335,7 +9595,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>307</v>
       </c>
@@ -9352,7 +9612,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>398</v>
       </c>
@@ -9369,7 +9629,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>401</v>
       </c>
@@ -9386,7 +9646,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>428</v>
       </c>
@@ -9400,7 +9660,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>429</v>
       </c>
@@ -9414,7 +9674,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>430</v>
       </c>
@@ -9428,7 +9688,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>431</v>
       </c>
@@ -9442,7 +9702,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>432</v>
       </c>
@@ -9456,7 +9716,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>433</v>
       </c>
@@ -9470,7 +9730,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>408</v>
       </c>
@@ -9484,7 +9744,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>312</v>
       </c>
@@ -9504,7 +9764,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>316</v>
       </c>
@@ -9521,7 +9781,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>318</v>
       </c>
@@ -9538,7 +9798,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>317</v>
       </c>
@@ -9552,7 +9812,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>321</v>
       </c>
@@ -9569,7 +9829,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>322</v>
       </c>
@@ -9586,7 +9846,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>323</v>
       </c>
@@ -9603,7 +9863,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>324</v>
       </c>
@@ -9617,7 +9877,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>325</v>
       </c>
@@ -9634,7 +9894,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>326</v>
       </c>
@@ -9651,7 +9911,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>327</v>
       </c>
@@ -9668,7 +9928,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>328</v>
       </c>
@@ -9682,7 +9942,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>329</v>
       </c>
@@ -9699,7 +9959,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>330</v>
       </c>
@@ -9716,7 +9976,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>331</v>
       </c>
@@ -9733,7 +9993,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>332</v>
       </c>
@@ -9747,7 +10007,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>333</v>
       </c>
@@ -9764,7 +10024,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>334</v>
       </c>
@@ -9781,7 +10041,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>335</v>
       </c>
@@ -9798,7 +10058,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>336</v>
       </c>
@@ -9812,7 +10072,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>358</v>
       </c>
@@ -9826,7 +10086,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>360</v>
       </c>
@@ -9840,7 +10100,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>363</v>
       </c>
@@ -9854,7 +10114,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>365</v>
       </c>
@@ -9868,7 +10128,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>367</v>
       </c>
@@ -9882,7 +10142,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>369</v>
       </c>
@@ -9896,7 +10156,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="59" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>372</v>
       </c>
@@ -9913,7 +10173,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>376</v>
       </c>
@@ -9930,7 +10190,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="61" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>379</v>
       </c>
@@ -9947,7 +10207,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>382</v>
       </c>
@@ -9964,7 +10224,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="63" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>385</v>
       </c>
@@ -9981,7 +10241,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="64" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>388</v>
       </c>
@@ -9995,7 +10255,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>390</v>
       </c>
@@ -10009,7 +10269,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>392</v>
       </c>
@@ -10023,7 +10283,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>394</v>
       </c>
@@ -10037,7 +10297,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>396</v>
       </c>
@@ -10051,7 +10311,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>402</v>
       </c>
@@ -10068,7 +10328,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>406</v>
       </c>
@@ -10082,7 +10342,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>411</v>
       </c>
@@ -10099,7 +10359,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>415</v>
       </c>
@@ -10113,7 +10373,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>418</v>
       </c>
@@ -10124,7 +10384,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>420</v>
       </c>
@@ -10138,7 +10398,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>423</v>
       </c>
@@ -10152,7 +10412,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>425</v>
       </c>
@@ -10177,15 +10437,15 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>441</v>
       </c>
@@ -10199,7 +10459,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>402</v>
       </c>
@@ -10213,7 +10473,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>446</v>
       </c>
@@ -10224,7 +10484,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>449</v>
       </c>
@@ -10235,7 +10495,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>452</v>
       </c>
@@ -10246,7 +10506,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>454</v>
       </c>
@@ -10257,7 +10517,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>457</v>
       </c>
@@ -10268,7 +10528,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>459</v>
       </c>
@@ -10279,7 +10539,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>461</v>
       </c>
@@ -10290,7 +10550,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>463</v>
       </c>
@@ -10304,7 +10564,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>466</v>
       </c>
@@ -10318,7 +10578,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>469</v>
       </c>
@@ -10329,7 +10589,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>471</v>
       </c>
@@ -10340,7 +10600,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>473</v>
       </c>
@@ -10351,7 +10611,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>266</v>
       </c>
@@ -10365,7 +10625,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>477</v>
       </c>
@@ -10376,7 +10636,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>479</v>
       </c>
@@ -10387,7 +10647,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>481</v>
       </c>
@@ -10398,7 +10658,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>483</v>
       </c>
@@ -10409,7 +10669,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>485</v>
       </c>
@@ -10420,7 +10680,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>487</v>
       </c>
@@ -10431,7 +10691,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>490</v>
       </c>
@@ -10442,7 +10702,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>312</v>
       </c>
@@ -10456,7 +10716,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>494</v>
       </c>
@@ -10467,7 +10727,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>496</v>
       </c>
@@ -10478,7 +10738,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>498</v>
       </c>
@@ -10489,7 +10749,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>500</v>
       </c>
@@ -10500,7 +10760,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>503</v>
       </c>
@@ -10511,7 +10771,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>505</v>
       </c>
@@ -10522,7 +10782,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>507</v>
       </c>
@@ -10533,7 +10793,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>509</v>
       </c>
@@ -10544,7 +10804,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>511</v>
       </c>
@@ -10555,7 +10815,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>512</v>
       </c>
@@ -10566,7 +10826,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>515</v>
       </c>
@@ -10580,7 +10840,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>519</v>
       </c>
@@ -10591,7 +10851,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>520</v>
       </c>
@@ -10602,7 +10862,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>521</v>
       </c>
@@ -10613,7 +10873,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>525</v>
       </c>
@@ -10627,7 +10887,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>528</v>
       </c>
@@ -10652,20 +10912,20 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" style="6" customWidth="1"/>
     <col min="6" max="6" width="41" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41" style="6" customWidth="1"/>
     <col min="8" max="8" width="15" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="6"/>
+    <col min="9" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>531</v>
       </c>
@@ -10691,7 +10951,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>411</v>
       </c>
@@ -10720,7 +10980,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" s="6">
         <v>1</v>
       </c>
@@ -10743,7 +11003,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>540</v>
       </c>
@@ -10760,7 +11020,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>542</v>
       </c>
@@ -10774,7 +11034,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>418</v>
       </c>
@@ -10788,7 +11048,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>545</v>
       </c>
@@ -10814,7 +11074,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>556</v>
       </c>
@@ -10840,7 +11100,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C9" s="6">
         <v>3000</v>
       </c>
@@ -10860,7 +11120,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C10" s="6">
         <v>4000</v>
       </c>
@@ -10880,7 +11140,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C11" s="6">
         <v>500</v>
       </c>
@@ -10900,7 +11160,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>572</v>
       </c>
@@ -10914,7 +11174,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" s="6">
         <v>2000</v>
       </c>
@@ -10922,7 +11182,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="6">
         <v>4000</v>
       </c>
@@ -10930,7 +11190,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>573</v>
       </c>
@@ -10947,7 +11207,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="6" t="s">
         <v>575</v>
       </c>
@@ -10961,7 +11221,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>579</v>
       </c>
@@ -10969,7 +11229,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>580</v>
       </c>
@@ -10980,7 +11240,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C19" s="6" t="s">
         <v>584</v>
       </c>
@@ -10988,7 +11248,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C20" s="6" t="s">
         <v>586</v>
       </c>
@@ -10996,7 +11256,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C21" s="6" t="s">
         <v>588</v>
       </c>
@@ -11004,7 +11264,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C22" s="6" t="s">
         <v>590</v>
       </c>
@@ -11012,7 +11272,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C23" s="6" t="s">
         <v>592</v>
       </c>
@@ -11020,7 +11280,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C24" s="6" t="s">
         <v>594</v>
       </c>
@@ -11028,7 +11288,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C25" s="6" t="s">
         <v>596</v>
       </c>
@@ -11036,7 +11296,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C26" s="6" t="s">
         <v>598</v>
       </c>
@@ -11044,7 +11304,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" s="6" t="s">
         <v>600</v>
       </c>
@@ -11052,7 +11312,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>602</v>
       </c>
@@ -11063,7 +11323,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C29" s="6">
         <v>1</v>
       </c>
@@ -11085,17 +11345,17 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="9"/>
-    <col min="5" max="5" width="42.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="9"/>
+    <col min="5" max="5" width="42.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>531</v>
       </c>
@@ -11115,7 +11375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>411</v>
       </c>
@@ -11132,7 +11392,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>418</v>
       </c>
@@ -11146,7 +11406,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>610</v>
       </c>
@@ -11163,7 +11423,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>530</v>
       </c>
@@ -11180,7 +11440,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>542</v>
       </c>
@@ -11194,7 +11454,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>545</v>
       </c>
@@ -11204,34 +11464,34 @@
       <c r="D7" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="18" t="s">
         <v>621</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="9" t="s">
         <v>617</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="18"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="18"/>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="9" t="s">
         <v>618</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E9" s="18"/>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>540</v>
       </c>
@@ -11248,7 +11508,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>556</v>
       </c>
@@ -11268,7 +11528,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>572</v>
       </c>
@@ -11285,7 +11545,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>573</v>
       </c>
@@ -11302,7 +11562,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>629</v>
       </c>
@@ -11315,28 +11575,28 @@
       <c r="D14" s="9" t="s">
         <v>619</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="18" t="s">
         <v>632</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="17" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="9" t="s">
         <v>631</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>619</v>
       </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="18"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E16" s="20"/>
-      <c r="F16" s="18"/>
-    </row>
-    <row r="17" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E15" s="18"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="18"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>633</v>
       </c>
@@ -11353,7 +11613,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
         <v>635</v>
       </c>
@@ -11367,7 +11627,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
         <v>602</v>
       </c>
@@ -11381,7 +11641,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>639</v>
       </c>
@@ -11395,7 +11655,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
         <v>642</v>
       </c>
@@ -11409,7 +11669,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
         <v>645</v>
       </c>
@@ -11423,7 +11683,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
         <v>648</v>
       </c>
@@ -11437,7 +11697,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
         <v>651</v>
       </c>
@@ -11454,7 +11714,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
         <v>580</v>
       </c>
@@ -11464,24 +11724,24 @@
       <c r="D25" s="9" t="s">
         <v>517</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="18" t="s">
         <v>654</v>
       </c>
-      <c r="F25" s="18" t="s">
+      <c r="F25" s="17" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C26" s="9" t="s">
         <v>640</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>517</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="18"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="18"/>
+      <c r="F26" s="17"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
         <v>655</v>
       </c>
@@ -11491,32 +11751,32 @@
       <c r="D27" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="18" t="s">
         <v>657</v>
       </c>
-      <c r="F27" s="18" t="s">
+      <c r="F27" s="17" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C28" s="9" t="s">
         <v>617</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="18"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E28" s="18"/>
+      <c r="F28" s="17"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C29" s="9" t="s">
         <v>656</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Closes #18, closes #22, closes #17, closes #19, closes #27, closes #25, closes #23, closes lo-co/exscalabar#26, closes lo-co/exscalabar#23, and closes lo-co/exscalabar#18.
</commit_message>
<xml_diff>
--- a/Support/Signal List.xlsx
+++ b/Support/Signal List.xlsx
@@ -3830,24 +3830,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4131,8 +4131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5353,7 +5353,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="19" t="s">
         <v>704</v>
       </c>
       <c r="C44" s="1"/>
@@ -5366,21 +5366,21 @@
       <c r="F44" s="1">
         <v>0</v>
       </c>
-      <c r="G44" s="17">
+      <c r="G44" s="20">
         <v>6225</v>
       </c>
-      <c r="H44" s="17" t="s">
+      <c r="H44" s="20" t="s">
         <v>114</v>
       </c>
       <c r="I44" s="1">
         <v>6</v>
       </c>
-      <c r="J44" s="19" t="s">
+      <c r="J44" s="23" t="s">
         <v>795</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="20"/>
+      <c r="B45" s="19"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
         <v>698</v>
@@ -5391,12 +5391,12 @@
       <c r="F45" s="1">
         <v>0</v>
       </c>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
       <c r="I45" s="1">
         <v>6</v>
       </c>
-      <c r="J45" s="19"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -5412,16 +5412,16 @@
       <c r="F46" s="1">
         <v>0</v>
       </c>
-      <c r="G46" s="17">
+      <c r="G46" s="20">
         <v>6225</v>
       </c>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="20" t="s">
         <v>114</v>
       </c>
       <c r="I46" s="1">
         <v>7</v>
       </c>
-      <c r="J46" s="18" t="s">
+      <c r="J46" s="22" t="s">
         <v>796</v>
       </c>
     </row>
@@ -5433,12 +5433,12 @@
       <c r="F47" s="1">
         <v>0</v>
       </c>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
       <c r="I47" s="1">
         <v>7</v>
       </c>
-      <c r="J47" s="18"/>
+      <c r="J47" s="22"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B48" s="21" t="s">
@@ -5455,7 +5455,7 @@
       <c r="I48" s="1">
         <v>7</v>
       </c>
-      <c r="J48" s="18" t="s">
+      <c r="J48" s="22" t="s">
         <v>803</v>
       </c>
     </row>
@@ -5472,7 +5472,7 @@
       <c r="I49" s="1">
         <v>7</v>
       </c>
-      <c r="J49" s="18"/>
+      <c r="J49" s="22"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="21" t="s">
@@ -5484,16 +5484,16 @@
       <c r="F50" s="1">
         <v>0</v>
       </c>
-      <c r="G50" s="17">
+      <c r="G50" s="20">
         <v>6225</v>
       </c>
-      <c r="H50" s="17" t="s">
+      <c r="H50" s="20" t="s">
         <v>114</v>
       </c>
       <c r="I50" s="1">
         <v>7</v>
       </c>
-      <c r="J50" s="18" t="s">
+      <c r="J50" s="22" t="s">
         <v>793</v>
       </c>
     </row>
@@ -5505,12 +5505,12 @@
       <c r="F51" s="1">
         <v>0</v>
       </c>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
       <c r="I51" s="1">
         <v>7</v>
       </c>
-      <c r="J51" s="18"/>
+      <c r="J51" s="22"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="21" t="s">
@@ -5527,7 +5527,7 @@
       <c r="I52" s="1">
         <v>7</v>
       </c>
-      <c r="J52" s="18" t="s">
+      <c r="J52" s="22" t="s">
         <v>804</v>
       </c>
     </row>
@@ -5544,7 +5544,7 @@
       <c r="I53" s="1">
         <v>7</v>
       </c>
-      <c r="J53" s="18"/>
+      <c r="J53" s="22"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
@@ -5919,7 +5919,7 @@
         <v>846</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>806</v>
+        <v>862</v>
       </c>
       <c r="E70" t="s">
         <v>858</v>
@@ -5934,7 +5934,7 @@
         <v>114</v>
       </c>
       <c r="I70" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J70" t="s">
         <v>853</v>
@@ -5960,7 +5960,7 @@
         <v>114</v>
       </c>
       <c r="I71" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J71" t="s">
         <v>852</v>
@@ -5986,35 +5986,35 @@
         <v>114</v>
       </c>
       <c r="I72" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J72" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="73" spans="1:10" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="22" t="s">
+    <row r="73" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="17" t="s">
         <v>839</v>
       </c>
-      <c r="D73" s="23" t="s">
+      <c r="D73" s="18" t="s">
         <v>840</v>
       </c>
-      <c r="E73" s="22" t="s">
+      <c r="E73" s="17" t="s">
         <v>830</v>
       </c>
-      <c r="F73" s="23">
+      <c r="F73" s="18">
         <v>0</v>
       </c>
-      <c r="G73" s="23">
+      <c r="G73" s="18">
         <v>6225</v>
       </c>
-      <c r="H73" s="23" t="s">
+      <c r="H73" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="I73" s="23">
+      <c r="I73" s="18">
         <v>6</v>
       </c>
-      <c r="J73" s="22" t="s">
+      <c r="J73" s="17" t="s">
         <v>860</v>
       </c>
     </row>
@@ -6022,7 +6022,7 @@
       <c r="A74" t="s">
         <v>266</v>
       </c>
-      <c r="B74" s="20" t="s">
+      <c r="B74" s="19" t="s">
         <v>719</v>
       </c>
       <c r="C74" s="1"/>
@@ -6047,7 +6047,7 @@
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B75" s="20"/>
+      <c r="B75" s="19"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
         <v>67</v>
@@ -6070,7 +6070,7 @@
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B76" s="20"/>
+      <c r="B76" s="19"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
         <v>68</v>
@@ -6093,7 +6093,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B77" s="20"/>
+      <c r="B77" s="19"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
         <v>69</v>
@@ -6191,7 +6191,7 @@
       </c>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B81" s="20" t="s">
+      <c r="B81" s="19" t="s">
         <v>723</v>
       </c>
       <c r="C81" s="1"/>
@@ -6214,7 +6214,7 @@
       <c r="J81" s="3"/>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B82" s="20"/>
+      <c r="B82" s="19"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
         <v>699</v>
@@ -6235,7 +6235,7 @@
       <c r="J82" s="3"/>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B83" s="20"/>
+      <c r="B83" s="19"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
         <v>700</v>
@@ -6256,7 +6256,7 @@
       <c r="J83" s="3"/>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B84" s="20"/>
+      <c r="B84" s="19"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
         <v>701</v>
@@ -6277,7 +6277,7 @@
       <c r="J84" s="3"/>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B85" s="20"/>
+      <c r="B85" s="19"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
         <v>702</v>
@@ -6318,7 +6318,7 @@
       </c>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B87" s="20" t="s">
+      <c r="B87" s="19" t="s">
         <v>725</v>
       </c>
       <c r="C87" s="1"/>
@@ -6341,7 +6341,7 @@
       </c>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B88" s="20"/>
+      <c r="B88" s="19"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
         <v>703</v>
@@ -6399,6 +6399,14 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="H46:H47"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="J46:J47"/>
     <mergeCell ref="B87:B88"/>
     <mergeCell ref="G44:G45"/>
     <mergeCell ref="B46:B47"/>
@@ -6410,14 +6418,6 @@
     <mergeCell ref="G50:G51"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="B52:B53"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="H46:H47"/>
-    <mergeCell ref="H50:H51"/>
-    <mergeCell ref="J48:J49"/>
-    <mergeCell ref="J52:J53"/>
-    <mergeCell ref="J50:J51"/>
-    <mergeCell ref="J44:J45"/>
-    <mergeCell ref="J46:J47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -9155,7 +9155,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="19" t="s">
         <v>704</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -9172,7 +9172,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="19"/>
       <c r="C18" s="1" t="s">
         <v>708</v>
       </c>
@@ -11464,10 +11464,10 @@
       <c r="D7" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="22" t="s">
         <v>621</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="20" t="s">
         <v>658</v>
       </c>
     </row>
@@ -11478,8 +11478,8 @@
       <c r="D8" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="17"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="9" t="s">
@@ -11488,8 +11488,8 @@
       <c r="D9" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="17"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
@@ -11575,10 +11575,10 @@
       <c r="D14" s="9" t="s">
         <v>619</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="22" t="s">
         <v>632</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="20" t="s">
         <v>658</v>
       </c>
     </row>
@@ -11589,12 +11589,12 @@
       <c r="D15" s="9" t="s">
         <v>619</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="17"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E16" s="18"/>
-      <c r="F16" s="17"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
@@ -11724,10 +11724,10 @@
       <c r="D25" s="9" t="s">
         <v>517</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="22" t="s">
         <v>654</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="20" t="s">
         <v>658</v>
       </c>
     </row>
@@ -11738,8 +11738,8 @@
       <c r="D26" s="9" t="s">
         <v>517</v>
       </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="17"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="20"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
@@ -11751,10 +11751,10 @@
       <c r="D27" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="22" t="s">
         <v>657</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="20" t="s">
         <v>658</v>
       </c>
     </row>
@@ -11765,8 +11765,8 @@
       <c r="D28" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="17"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="20"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C29" s="9" t="s">
@@ -11775,8 +11775,8 @@
       <c r="D29" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="17"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Associated with fix of issue #33.
</commit_message>
<xml_diff>
--- a/Support/Signal List.xlsx
+++ b/Support/Signal List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9645" windowHeight="3870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9648" windowHeight="3876"/>
   </bookViews>
   <sheets>
     <sheet name="DAQ Signals All" sheetId="11" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="867">
   <si>
     <t>Speaker Out</t>
   </si>
@@ -3680,18 +3680,12 @@
     <t>TEC PS Enable</t>
   </si>
   <si>
-    <t>Sample Pump Block</t>
-  </si>
-  <si>
     <t>Laser Interlock</t>
   </si>
   <si>
     <t>P1.2</t>
   </si>
   <si>
-    <t>Blocked Impactor</t>
-  </si>
-  <si>
     <t>P1.3</t>
   </si>
   <si>
@@ -3701,9 +3695,6 @@
     <t>Input from laser enclosure interlock</t>
   </si>
   <si>
-    <t>Input from sample pump indicating blockage</t>
-  </si>
-  <si>
     <t>51,18</t>
   </si>
   <si>
@@ -3729,6 +3720,27 @@
   </si>
   <si>
     <t>P1.4</t>
+  </si>
+  <si>
+    <t>Purge Switch</t>
+  </si>
+  <si>
+    <t>P1.5</t>
+  </si>
+  <si>
+    <t>High is flow through MFC; low is through critical orifice.</t>
+  </si>
+  <si>
+    <t>Differential pressure measurement on sample pump.  High value (TBD) indicates that pump is blocked</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>Impactor Differential Pressure</t>
+  </si>
+  <si>
+    <t>Sample pump blocked</t>
   </si>
 </sst>
 </file>
@@ -3786,7 +3798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3832,6 +3844,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4129,27 +4145,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="75.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="75.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>713</v>
       </c>
@@ -4181,7 +4197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>312</v>
       </c>
@@ -4213,7 +4229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
@@ -4242,7 +4258,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
@@ -4271,7 +4287,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
@@ -4300,7 +4316,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -4329,7 +4345,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
@@ -4358,7 +4374,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
@@ -4387,7 +4403,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
@@ -4416,7 +4432,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>35</v>
       </c>
@@ -4445,7 +4461,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>37</v>
       </c>
@@ -4474,7 +4490,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
@@ -4503,7 +4519,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>41</v>
       </c>
@@ -4532,7 +4548,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>51</v>
       </c>
@@ -4561,7 +4577,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>53</v>
       </c>
@@ -4590,7 +4606,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>54</v>
       </c>
@@ -4619,7 +4635,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>55</v>
       </c>
@@ -4648,7 +4664,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>56</v>
       </c>
@@ -4677,7 +4693,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>170</v>
       </c>
@@ -4704,7 +4720,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>171</v>
       </c>
@@ -4731,7 +4747,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>172</v>
       </c>
@@ -4758,7 +4774,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>173</v>
       </c>
@@ -4785,7 +4801,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>174</v>
       </c>
@@ -4812,7 +4828,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>73</v>
       </c>
@@ -4839,7 +4855,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>74</v>
       </c>
@@ -4866,7 +4882,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>75</v>
       </c>
@@ -4893,7 +4909,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>76</v>
       </c>
@@ -4920,7 +4936,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>77</v>
       </c>
@@ -4947,7 +4963,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
         <v>80</v>
       </c>
@@ -4974,7 +4990,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>81</v>
       </c>
@@ -5001,7 +5017,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>83</v>
       </c>
@@ -5028,7 +5044,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>84</v>
       </c>
@@ -5055,7 +5071,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>85</v>
       </c>
@@ -5082,7 +5098,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>94</v>
       </c>
@@ -5109,7 +5125,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
         <v>95</v>
       </c>
@@ -5136,7 +5152,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
         <v>96</v>
       </c>
@@ -5163,7 +5179,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
         <v>97</v>
       </c>
@@ -5190,7 +5206,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
         <v>98</v>
       </c>
@@ -5217,7 +5233,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
         <v>104</v>
       </c>
@@ -5244,7 +5260,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B40" s="3" t="s">
         <v>105</v>
       </c>
@@ -5271,7 +5287,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B41" s="3" t="s">
         <v>106</v>
       </c>
@@ -5298,7 +5314,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="s">
         <v>107</v>
       </c>
@@ -5325,7 +5341,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
         <v>108</v>
       </c>
@@ -5352,8 +5368,8 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="19" t="s">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="21" t="s">
         <v>704</v>
       </c>
       <c r="C44" s="1"/>
@@ -5366,21 +5382,21 @@
       <c r="F44" s="1">
         <v>0</v>
       </c>
-      <c r="G44" s="20">
+      <c r="G44" s="22">
         <v>6225</v>
       </c>
-      <c r="H44" s="20" t="s">
+      <c r="H44" s="22" t="s">
         <v>114</v>
       </c>
       <c r="I44" s="1">
         <v>6</v>
       </c>
-      <c r="J44" s="23" t="s">
+      <c r="J44" s="25" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="19"/>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B45" s="21"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
         <v>698</v>
@@ -5391,18 +5407,18 @@
       <c r="F45" s="1">
         <v>0</v>
       </c>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
       <c r="I45" s="1">
         <v>6</v>
       </c>
-      <c r="J45" s="23"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J45" s="25"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>411</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="23" t="s">
         <v>797</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -5412,36 +5428,36 @@
       <c r="F46" s="1">
         <v>0</v>
       </c>
-      <c r="G46" s="20">
+      <c r="G46" s="22">
         <v>6225</v>
       </c>
-      <c r="H46" s="20" t="s">
+      <c r="H46" s="22" t="s">
         <v>114</v>
       </c>
       <c r="I46" s="1">
         <v>7</v>
       </c>
-      <c r="J46" s="22" t="s">
+      <c r="J46" s="24" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="21"/>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B47" s="23"/>
       <c r="D47" s="1" t="s">
         <v>698</v>
       </c>
       <c r="F47" s="1">
         <v>0</v>
       </c>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
       <c r="I47" s="1">
         <v>7</v>
       </c>
-      <c r="J47" s="22"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="21" t="s">
+      <c r="J47" s="24"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B48" s="23" t="s">
         <v>799</v>
       </c>
       <c r="D48" s="1" t="s">
@@ -5455,12 +5471,12 @@
       <c r="I48" s="1">
         <v>7</v>
       </c>
-      <c r="J48" s="22" t="s">
+      <c r="J48" s="24" t="s">
         <v>803</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="21"/>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B49" s="23"/>
       <c r="D49" s="1" t="s">
         <v>801</v>
       </c>
@@ -5472,10 +5488,10 @@
       <c r="I49" s="1">
         <v>7</v>
       </c>
-      <c r="J49" s="22"/>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="21" t="s">
+      <c r="J49" s="24"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B50" s="23" t="s">
         <v>798</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -5484,36 +5500,36 @@
       <c r="F50" s="1">
         <v>0</v>
       </c>
-      <c r="G50" s="20">
+      <c r="G50" s="22">
         <v>6225</v>
       </c>
-      <c r="H50" s="20" t="s">
+      <c r="H50" s="22" t="s">
         <v>114</v>
       </c>
       <c r="I50" s="1">
         <v>7</v>
       </c>
-      <c r="J50" s="22" t="s">
+      <c r="J50" s="24" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="21"/>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B51" s="23"/>
       <c r="D51" s="1" t="s">
         <v>705</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
       </c>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
       <c r="I51" s="1">
         <v>7</v>
       </c>
-      <c r="J51" s="22"/>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="21" t="s">
+      <c r="J51" s="24"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B52" s="23" t="s">
         <v>802</v>
       </c>
       <c r="D52" s="1" t="s">
@@ -5527,12 +5543,12 @@
       <c r="I52" s="1">
         <v>7</v>
       </c>
-      <c r="J52" s="22" t="s">
+      <c r="J52" s="24" t="s">
         <v>804</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="21"/>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B53" s="23"/>
       <c r="D53" s="1" t="s">
         <v>806</v>
       </c>
@@ -5544,9 +5560,9 @@
       <c r="I53" s="1">
         <v>7</v>
       </c>
-      <c r="J53" s="22"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J53" s="24"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>707</v>
       </c>
@@ -5569,15 +5585,15 @@
         <v>794</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>810</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="E55" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="F55" s="1">
         <v>0</v>
@@ -5592,7 +5608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>818</v>
       </c>
@@ -5615,7 +5631,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>819</v>
       </c>
@@ -5638,7 +5654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>820</v>
       </c>
@@ -5661,7 +5677,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>821</v>
       </c>
@@ -5684,7 +5700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>822</v>
       </c>
@@ -5707,7 +5723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>823</v>
       </c>
@@ -5730,7 +5746,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>824</v>
       </c>
@@ -5753,7 +5769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>825</v>
       </c>
@@ -5776,7 +5792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>826</v>
       </c>
@@ -5799,7 +5815,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>827</v>
       </c>
@@ -5822,7 +5838,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>841</v>
       </c>
@@ -5830,7 +5846,7 @@
         <v>800</v>
       </c>
       <c r="E66" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="F66" s="1">
         <v>0</v>
@@ -5845,7 +5861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>842</v>
       </c>
@@ -5853,7 +5869,7 @@
         <v>801</v>
       </c>
       <c r="E67" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="F67" s="1">
         <v>0</v>
@@ -5868,7 +5884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>843</v>
       </c>
@@ -5876,7 +5892,7 @@
         <v>844</v>
       </c>
       <c r="E68" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="F68" s="1">
         <v>0</v>
@@ -5891,7 +5907,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>845</v>
       </c>
@@ -5899,7 +5915,7 @@
         <v>805</v>
       </c>
       <c r="E69" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="F69" s="1">
         <v>0</v>
@@ -5914,15 +5930,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>846</v>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B70" s="3" t="s">
+        <v>860</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="E70" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="F70" s="1">
         <v>0</v>
@@ -5937,18 +5953,18 @@
         <v>7</v>
       </c>
       <c r="J70" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
+        <v>846</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>847</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>848</v>
-      </c>
       <c r="E71" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="F71" s="1">
         <v>0</v>
@@ -5963,15 +5979,15 @@
         <v>7</v>
       </c>
       <c r="J71" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
-        <v>849</v>
+        <v>866</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="E72" t="s">
         <v>58</v>
@@ -5989,10 +6005,10 @@
         <v>7</v>
       </c>
       <c r="J72" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B73" s="17" t="s">
         <v>839</v>
       </c>
@@ -6015,45 +6031,48 @@
         <v>6</v>
       </c>
       <c r="J73" s="17" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="19" t="s">
+        <v>865</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="F74" s="20">
+        <v>0</v>
+      </c>
+      <c r="G74" s="20">
+        <v>6225</v>
+      </c>
+      <c r="H74" s="20" t="s">
+        <v>864</v>
+      </c>
+      <c r="I74" s="20">
+        <v>7</v>
+      </c>
+      <c r="J74" s="19" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>266</v>
       </c>
-      <c r="B74" s="19" t="s">
+      <c r="B75" s="21" t="s">
         <v>719</v>
       </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F74" s="1">
-        <v>0</v>
-      </c>
-      <c r="G74" s="1">
-        <v>6124</v>
-      </c>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1">
-        <v>3</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B75" s="19"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>231</v>
+        <v>175</v>
       </c>
       <c r="F75" s="1">
         <v>0</v>
@@ -6066,17 +6085,17 @@
         <v>3</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B76" s="19"/>
+        <v>717</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B76" s="21"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>177</v>
+        <v>231</v>
       </c>
       <c r="F76" s="1">
         <v>0</v>
@@ -6089,17 +6108,17 @@
         <v>3</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B77" s="19"/>
+        <v>718</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B77" s="21"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>232</v>
+        <v>177</v>
       </c>
       <c r="F77" s="1">
         <v>0</v>
@@ -6112,69 +6131,67 @@
         <v>3</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B78" s="3" t="s">
-        <v>720</v>
-      </c>
+        <v>715</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B78" s="21"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>175</v>
+        <v>232</v>
       </c>
       <c r="F78" s="1">
         <v>0</v>
       </c>
       <c r="G78" s="1">
-        <v>6132</v>
+        <v>6124</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B79" s="3" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="F79" s="1">
         <v>0</v>
       </c>
       <c r="G79" s="1">
-        <v>6225</v>
+        <v>6132</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B80" s="3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>233</v>
+        <v>160</v>
       </c>
       <c r="F80" s="1">
         <v>0</v>
@@ -6187,40 +6204,44 @@
         <v>8</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B81" s="19" t="s">
-        <v>723</v>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B81" s="3" t="s">
+        <v>722</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>111</v>
+        <v>233</v>
+      </c>
+      <c r="F81" s="1">
+        <v>0</v>
       </c>
       <c r="G81" s="1">
-        <v>6704</v>
+        <v>6225</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1">
-        <v>6</v>
-      </c>
-      <c r="J81" s="3"/>
-    </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B82" s="19"/>
+        <v>8</v>
+      </c>
+      <c r="J81" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B82" s="21" t="s">
+        <v>723</v>
+      </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>699</v>
+        <v>23</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>111</v>
@@ -6234,14 +6255,14 @@
       </c>
       <c r="J82" s="3"/>
     </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B83" s="19"/>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B83" s="21"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>111</v>
@@ -6255,14 +6276,14 @@
       </c>
       <c r="J83" s="3"/>
     </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B84" s="19"/>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B84" s="21"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>111</v>
@@ -6276,14 +6297,14 @@
       </c>
       <c r="J84" s="3"/>
     </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B85" s="19"/>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B85" s="21"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>15</v>
+        <v>237</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>111</v>
@@ -6297,38 +6318,36 @@
       </c>
       <c r="J85" s="3"/>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B86" s="3" t="s">
-        <v>724</v>
-      </c>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B86" s="21"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>697</v>
-      </c>
-      <c r="E86" s="1"/>
+        <v>702</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="G86" s="1">
-        <v>6225</v>
+        <v>6704</v>
       </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1">
-        <v>7</v>
-      </c>
-      <c r="J86" s="3" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B87" s="19" t="s">
-        <v>725</v>
+        <v>6</v>
+      </c>
+      <c r="J86" s="3"/>
+    </row>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B87" s="3" t="s">
+        <v>724</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E87" s="1"/>
-      <c r="F87" s="1">
-        <v>0</v>
-      </c>
       <c r="G87" s="1">
         <v>6225</v>
       </c>
@@ -6337,14 +6356,16 @@
         <v>7</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B88" s="19"/>
+        <v>726</v>
+      </c>
+    </row>
+    <row r="88" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B88" s="21" t="s">
+        <v>725</v>
+      </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1">
@@ -6358,44 +6379,76 @@
         <v>7</v>
       </c>
       <c r="J88" s="3" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="89" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B89" s="21"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1">
+        <v>0</v>
+      </c>
+      <c r="G89" s="1">
+        <v>6225</v>
+      </c>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1">
+        <v>7</v>
+      </c>
+      <c r="J89" s="3" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B89" s="16" t="s">
+    <row r="90" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B90" s="16" t="s">
         <v>807</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G89" s="1">
-        <v>6704</v>
-      </c>
-    </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B90" s="16" t="s">
-        <v>808</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="G90" s="1">
         <v>6704</v>
       </c>
     </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B91" s="3" t="s">
-        <v>809</v>
-      </c>
-      <c r="C91" s="1"/>
+    <row r="91" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B91" s="16" t="s">
+        <v>808</v>
+      </c>
       <c r="D91" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E91" s="1"/>
+        <v>14</v>
+      </c>
       <c r="G91" s="1">
         <v>6704</v>
       </c>
-      <c r="H91" s="1"/>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B92" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E92" s="1"/>
+      <c r="G92" s="1">
+        <v>6704</v>
+      </c>
+      <c r="H92" s="1"/>
+    </row>
+    <row r="93" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B93" s="3" t="s">
+        <v>860</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="G93" s="1">
+        <v>6225</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -6407,13 +6460,13 @@
     <mergeCell ref="J50:J51"/>
     <mergeCell ref="J44:J45"/>
     <mergeCell ref="J46:J47"/>
-    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B88:B89"/>
     <mergeCell ref="G44:G45"/>
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="B81:B85"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="B82:B86"/>
     <mergeCell ref="G46:G47"/>
     <mergeCell ref="G50:G51"/>
     <mergeCell ref="B48:B49"/>
@@ -6432,12 +6485,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>312</v>
       </c>
@@ -6448,7 +6501,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>660</v>
       </c>
@@ -6456,7 +6509,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>509</v>
       </c>
@@ -6464,7 +6517,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>511</v>
       </c>
@@ -6472,7 +6525,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>512</v>
       </c>
@@ -6480,7 +6533,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>661</v>
       </c>
@@ -6488,7 +6541,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>662</v>
       </c>
@@ -6496,7 +6549,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>663</v>
       </c>
@@ -6504,7 +6557,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>664</v>
       </c>
@@ -6512,7 +6565,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>665</v>
       </c>
@@ -6520,7 +6573,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>666</v>
       </c>
@@ -6528,7 +6581,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>667</v>
       </c>
@@ -6536,7 +6589,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>668</v>
       </c>
@@ -6544,7 +6597,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>669</v>
       </c>
@@ -6552,7 +6605,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>670</v>
       </c>
@@ -6560,7 +6613,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>671</v>
       </c>
@@ -6568,7 +6621,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>266</v>
       </c>
@@ -6579,7 +6632,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>572</v>
       </c>
@@ -6587,7 +6640,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>672</v>
       </c>
@@ -6595,7 +6648,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>411</v>
       </c>
@@ -6606,7 +6659,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>674</v>
       </c>
@@ -6614,7 +6667,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>675</v>
       </c>
@@ -6622,7 +6675,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>676</v>
       </c>
@@ -6630,7 +6683,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>684</v>
       </c>
@@ -6638,7 +6691,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>677</v>
       </c>
@@ -6646,7 +6699,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>515</v>
       </c>
@@ -6654,22 +6707,22 @@
         <v>679</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>402</v>
       </c>
@@ -6677,17 +6730,17 @@
         <v>680</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>683</v>
       </c>
@@ -6695,17 +6748,17 @@
         <v>483</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>521</v>
       </c>
@@ -6723,12 +6776,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>690</v>
       </c>
@@ -6736,7 +6789,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>692</v>
       </c>
@@ -6757,17 +6810,17 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>250</v>
       </c>
@@ -6787,7 +6840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>729</v>
       </c>
@@ -6804,7 +6857,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D3" s="5" t="s">
         <v>731</v>
       </c>
@@ -6815,7 +6868,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D4" s="5" t="s">
         <v>732</v>
       </c>
@@ -6826,7 +6879,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D5" s="5" t="s">
         <v>733</v>
       </c>
@@ -6837,7 +6890,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D6" s="5" t="s">
         <v>734</v>
       </c>
@@ -6848,7 +6901,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>736</v>
       </c>
@@ -6862,7 +6915,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D8" s="5" t="s">
         <v>738</v>
       </c>
@@ -6873,7 +6926,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>709</v>
       </c>
@@ -6893,7 +6946,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D10" s="5" t="s">
         <v>748</v>
       </c>
@@ -6904,7 +6957,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" s="5" t="s">
         <v>749</v>
       </c>
@@ -6915,7 +6968,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="5" t="s">
         <v>521</v>
       </c>
@@ -6926,7 +6979,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D13" s="5" t="s">
         <v>750</v>
       </c>
@@ -6937,7 +6990,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" s="5" t="s">
         <v>751</v>
       </c>
@@ -6948,7 +7001,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" s="5" t="s">
         <v>752</v>
       </c>
@@ -6959,7 +7012,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" s="5" t="s">
         <v>753</v>
       </c>
@@ -6970,7 +7023,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D17" s="5" t="s">
         <v>754</v>
       </c>
@@ -6981,7 +7034,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D18" s="5" t="s">
         <v>755</v>
       </c>
@@ -6992,7 +7045,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>768</v>
       </c>
@@ -7006,7 +7059,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>771</v>
       </c>
@@ -7023,7 +7076,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D21" s="5" t="s">
         <v>731</v>
       </c>
@@ -7034,7 +7087,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D22" s="5" t="s">
         <v>732</v>
       </c>
@@ -7045,7 +7098,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>776</v>
       </c>
@@ -7062,7 +7115,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D24" s="5" t="s">
         <v>779</v>
       </c>
@@ -7073,7 +7126,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D25" s="5" t="s">
         <v>780</v>
       </c>
@@ -7084,7 +7137,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D26" s="5" t="s">
         <v>778</v>
       </c>
@@ -7095,7 +7148,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D27" s="5" t="s">
         <v>781</v>
       </c>
@@ -7106,7 +7159,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D28" s="5" t="s">
         <v>782</v>
       </c>
@@ -7117,7 +7170,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D29" s="5" t="s">
         <v>783</v>
       </c>
@@ -7128,7 +7181,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D30" s="5" t="s">
         <v>784</v>
       </c>
@@ -7139,7 +7192,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D31" s="5" t="s">
         <v>785</v>
       </c>
@@ -7163,22 +7216,22 @@
       <selection sqref="A1:J53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="6" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -7210,7 +7263,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -7242,7 +7295,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -7274,7 +7327,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -7306,7 +7359,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -7338,7 +7391,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -7370,7 +7423,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -7402,7 +7455,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -7434,7 +7487,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -7466,7 +7519,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
@@ -7498,7 +7551,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>37</v>
       </c>
@@ -7530,7 +7583,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>39</v>
       </c>
@@ -7562,7 +7615,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>41</v>
       </c>
@@ -7594,7 +7647,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
@@ -7626,7 +7679,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
@@ -7658,7 +7711,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>54</v>
       </c>
@@ -7690,7 +7743,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>55</v>
       </c>
@@ -7722,7 +7775,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>56</v>
       </c>
@@ -7754,7 +7807,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>170</v>
       </c>
@@ -7783,7 +7836,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>171</v>
       </c>
@@ -7812,7 +7865,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>172</v>
       </c>
@@ -7841,7 +7894,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>173</v>
       </c>
@@ -7870,7 +7923,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>174</v>
       </c>
@@ -7899,7 +7952,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>73</v>
       </c>
@@ -7925,7 +7978,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>74</v>
       </c>
@@ -7951,7 +8004,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>75</v>
       </c>
@@ -7977,7 +8030,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
@@ -8003,7 +8056,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>77</v>
       </c>
@@ -8029,7 +8082,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>80</v>
       </c>
@@ -8055,7 +8108,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>81</v>
       </c>
@@ -8081,7 +8134,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>83</v>
       </c>
@@ -8107,7 +8160,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>84</v>
       </c>
@@ -8133,7 +8186,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>85</v>
       </c>
@@ -8159,7 +8212,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>94</v>
       </c>
@@ -8185,7 +8238,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>95</v>
       </c>
@@ -8211,7 +8264,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>96</v>
       </c>
@@ -8237,7 +8290,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>97</v>
       </c>
@@ -8263,7 +8316,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>98</v>
       </c>
@@ -8289,7 +8342,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>104</v>
       </c>
@@ -8315,7 +8368,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>105</v>
       </c>
@@ -8341,7 +8394,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>106</v>
       </c>
@@ -8367,7 +8420,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>107</v>
       </c>
@@ -8393,7 +8446,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>108</v>
       </c>
@@ -8419,7 +8472,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>113</v>
       </c>
@@ -8445,7 +8498,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>115</v>
       </c>
@@ -8471,7 +8524,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>116</v>
       </c>
@@ -8497,7 +8550,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>117</v>
       </c>
@@ -8523,7 +8576,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>118</v>
       </c>
@@ -8549,7 +8602,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>119</v>
       </c>
@@ -8575,7 +8628,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>120</v>
       </c>
@@ -8601,7 +8654,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>121</v>
       </c>
@@ -8627,7 +8680,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>122</v>
       </c>
@@ -8653,7 +8706,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>123</v>
       </c>
@@ -8692,20 +8745,20 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -8734,8 +8787,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>466</v>
       </c>
       <c r="C2" t="s">
@@ -8748,8 +8801,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
       <c r="C3" t="s">
         <v>698</v>
       </c>
@@ -8760,8 +8813,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
         <v>706</v>
       </c>
       <c r="C4" t="s">
@@ -8774,8 +8827,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
       <c r="C5" t="s">
         <v>705</v>
       </c>
@@ -8786,7 +8839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>707</v>
       </c>
@@ -8817,21 +8870,21 @@
       <selection activeCell="A2" sqref="A2:I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -8860,7 +8913,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>247</v>
       </c>
@@ -8880,7 +8933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>239</v>
       </c>
@@ -8900,7 +8953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>240</v>
       </c>
@@ -8920,7 +8973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>241</v>
       </c>
@@ -8940,7 +8993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>242</v>
       </c>
@@ -8960,7 +9013,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>243</v>
       </c>
@@ -8983,7 +9036,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>244</v>
       </c>
@@ -9006,7 +9059,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>124</v>
       </c>
@@ -9026,7 +9079,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>125</v>
       </c>
@@ -9046,7 +9099,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>126</v>
       </c>
@@ -9066,7 +9119,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>127</v>
       </c>
@@ -9086,7 +9139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>128</v>
       </c>
@@ -9106,7 +9159,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>694</v>
       </c>
@@ -9120,7 +9173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>695</v>
       </c>
@@ -9137,7 +9190,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>696</v>
       </c>
@@ -9154,8 +9207,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
         <v>704</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -9171,8 +9224,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="21"/>
       <c r="C18" s="1" t="s">
         <v>708</v>
       </c>
@@ -9203,16 +9256,16 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>249</v>
       </c>
@@ -9232,7 +9285,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>248</v>
       </c>
@@ -9252,7 +9305,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>257</v>
       </c>
@@ -9269,7 +9322,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>258</v>
       </c>
@@ -9286,7 +9339,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>259</v>
       </c>
@@ -9303,7 +9356,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>260</v>
       </c>
@@ -9320,7 +9373,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>261</v>
       </c>
@@ -9337,7 +9390,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>262</v>
       </c>
@@ -9354,7 +9407,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>263</v>
       </c>
@@ -9371,7 +9424,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>264</v>
       </c>
@@ -9388,7 +9441,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>265</v>
       </c>
@@ -9405,7 +9458,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>283</v>
       </c>
@@ -9422,7 +9475,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>266</v>
       </c>
@@ -9442,7 +9495,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>302</v>
       </c>
@@ -9459,7 +9512,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>303</v>
       </c>
@@ -9476,7 +9529,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>304</v>
       </c>
@@ -9493,7 +9546,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>290</v>
       </c>
@@ -9510,7 +9563,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>293</v>
       </c>
@@ -9527,7 +9580,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>295</v>
       </c>
@@ -9544,7 +9597,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>297</v>
       </c>
@@ -9561,7 +9614,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>299</v>
       </c>
@@ -9578,7 +9631,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>305</v>
       </c>
@@ -9595,7 +9648,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>307</v>
       </c>
@@ -9612,7 +9665,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>398</v>
       </c>
@@ -9629,7 +9682,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>401</v>
       </c>
@@ -9646,7 +9699,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>428</v>
       </c>
@@ -9660,7 +9713,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>429</v>
       </c>
@@ -9674,7 +9727,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>430</v>
       </c>
@@ -9688,7 +9741,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>431</v>
       </c>
@@ -9702,7 +9755,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>432</v>
       </c>
@@ -9716,7 +9769,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>433</v>
       </c>
@@ -9730,7 +9783,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>408</v>
       </c>
@@ -9744,7 +9797,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>312</v>
       </c>
@@ -9764,7 +9817,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>316</v>
       </c>
@@ -9781,7 +9834,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>318</v>
       </c>
@@ -9798,7 +9851,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>317</v>
       </c>
@@ -9812,7 +9865,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>321</v>
       </c>
@@ -9829,7 +9882,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>322</v>
       </c>
@@ -9846,7 +9899,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>323</v>
       </c>
@@ -9863,7 +9916,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>324</v>
       </c>
@@ -9877,7 +9930,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>325</v>
       </c>
@@ -9894,7 +9947,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>326</v>
       </c>
@@ -9911,7 +9964,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>327</v>
       </c>
@@ -9928,7 +9981,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>328</v>
       </c>
@@ -9942,7 +9995,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>329</v>
       </c>
@@ -9959,7 +10012,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>330</v>
       </c>
@@ -9976,7 +10029,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>331</v>
       </c>
@@ -9993,7 +10046,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>332</v>
       </c>
@@ -10007,7 +10060,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>333</v>
       </c>
@@ -10024,7 +10077,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>334</v>
       </c>
@@ -10041,7 +10094,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>335</v>
       </c>
@@ -10058,7 +10111,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>336</v>
       </c>
@@ -10072,7 +10125,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>358</v>
       </c>
@@ -10086,7 +10139,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>360</v>
       </c>
@@ -10100,7 +10153,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>363</v>
       </c>
@@ -10114,7 +10167,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>365</v>
       </c>
@@ -10128,7 +10181,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>367</v>
       </c>
@@ -10142,7 +10195,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>369</v>
       </c>
@@ -10156,7 +10209,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="59" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>372</v>
       </c>
@@ -10173,7 +10226,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>376</v>
       </c>
@@ -10190,7 +10243,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="61" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>379</v>
       </c>
@@ -10207,7 +10260,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>382</v>
       </c>
@@ -10224,7 +10277,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="63" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>385</v>
       </c>
@@ -10241,7 +10294,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="64" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>388</v>
       </c>
@@ -10255,7 +10308,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>390</v>
       </c>
@@ -10269,7 +10322,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>392</v>
       </c>
@@ -10283,7 +10336,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>394</v>
       </c>
@@ -10297,7 +10350,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>396</v>
       </c>
@@ -10311,7 +10364,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>402</v>
       </c>
@@ -10328,7 +10381,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>406</v>
       </c>
@@ -10342,7 +10395,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>411</v>
       </c>
@@ -10359,7 +10412,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>415</v>
       </c>
@@ -10373,7 +10426,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>418</v>
       </c>
@@ -10384,7 +10437,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>420</v>
       </c>
@@ -10398,7 +10451,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>423</v>
       </c>
@@ -10412,7 +10465,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>425</v>
       </c>
@@ -10437,15 +10490,15 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>441</v>
       </c>
@@ -10459,7 +10512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>402</v>
       </c>
@@ -10473,7 +10526,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>446</v>
       </c>
@@ -10484,7 +10537,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>449</v>
       </c>
@@ -10495,7 +10548,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>452</v>
       </c>
@@ -10506,7 +10559,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>454</v>
       </c>
@@ -10517,7 +10570,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>457</v>
       </c>
@@ -10528,7 +10581,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>459</v>
       </c>
@@ -10539,7 +10592,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>461</v>
       </c>
@@ -10550,7 +10603,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>463</v>
       </c>
@@ -10564,7 +10617,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>466</v>
       </c>
@@ -10578,7 +10631,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>469</v>
       </c>
@@ -10589,7 +10642,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>471</v>
       </c>
@@ -10600,7 +10653,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>473</v>
       </c>
@@ -10611,7 +10664,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>266</v>
       </c>
@@ -10625,7 +10678,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>477</v>
       </c>
@@ -10636,7 +10689,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>479</v>
       </c>
@@ -10647,7 +10700,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>481</v>
       </c>
@@ -10658,7 +10711,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>483</v>
       </c>
@@ -10669,7 +10722,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>485</v>
       </c>
@@ -10680,7 +10733,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>487</v>
       </c>
@@ -10691,7 +10744,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>490</v>
       </c>
@@ -10702,7 +10755,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>312</v>
       </c>
@@ -10716,7 +10769,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>494</v>
       </c>
@@ -10727,7 +10780,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>496</v>
       </c>
@@ -10738,7 +10791,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>498</v>
       </c>
@@ -10749,7 +10802,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>500</v>
       </c>
@@ -10760,7 +10813,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>503</v>
       </c>
@@ -10771,7 +10824,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>505</v>
       </c>
@@ -10782,7 +10835,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>507</v>
       </c>
@@ -10793,7 +10846,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>509</v>
       </c>
@@ -10804,7 +10857,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>511</v>
       </c>
@@ -10815,7 +10868,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>512</v>
       </c>
@@ -10826,7 +10879,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>515</v>
       </c>
@@ -10840,7 +10893,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>519</v>
       </c>
@@ -10851,7 +10904,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>520</v>
       </c>
@@ -10862,7 +10915,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>521</v>
       </c>
@@ -10873,7 +10926,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>525</v>
       </c>
@@ -10887,7 +10940,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>528</v>
       </c>
@@ -10912,20 +10965,20 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" style="6" customWidth="1"/>
     <col min="6" max="6" width="41" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41" style="6" customWidth="1"/>
     <col min="8" max="8" width="15" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="6"/>
+    <col min="9" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>531</v>
       </c>
@@ -10951,7 +11004,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>411</v>
       </c>
@@ -10980,7 +11033,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C3" s="6">
         <v>1</v>
       </c>
@@ -11003,7 +11056,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>540</v>
       </c>
@@ -11020,7 +11073,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>542</v>
       </c>
@@ -11034,7 +11087,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>418</v>
       </c>
@@ -11048,7 +11101,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>545</v>
       </c>
@@ -11074,7 +11127,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>556</v>
       </c>
@@ -11100,7 +11153,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C9" s="6">
         <v>3000</v>
       </c>
@@ -11120,7 +11173,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C10" s="6">
         <v>4000</v>
       </c>
@@ -11140,7 +11193,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C11" s="6">
         <v>500</v>
       </c>
@@ -11160,7 +11213,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>572</v>
       </c>
@@ -11174,7 +11227,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C13" s="6">
         <v>2000</v>
       </c>
@@ -11182,7 +11235,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C14" s="6">
         <v>4000</v>
       </c>
@@ -11190,7 +11243,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>573</v>
       </c>
@@ -11207,7 +11260,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C16" s="6" t="s">
         <v>575</v>
       </c>
@@ -11221,7 +11274,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
         <v>579</v>
       </c>
@@ -11229,7 +11282,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
         <v>580</v>
       </c>
@@ -11240,7 +11293,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C19" s="6" t="s">
         <v>584</v>
       </c>
@@ -11248,7 +11301,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C20" s="6" t="s">
         <v>586</v>
       </c>
@@ -11256,7 +11309,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C21" s="6" t="s">
         <v>588</v>
       </c>
@@ -11264,7 +11317,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C22" s="6" t="s">
         <v>590</v>
       </c>
@@ -11272,7 +11325,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C23" s="6" t="s">
         <v>592</v>
       </c>
@@ -11280,7 +11333,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C24" s="6" t="s">
         <v>594</v>
       </c>
@@ -11288,7 +11341,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C25" s="6" t="s">
         <v>596</v>
       </c>
@@ -11296,7 +11349,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C26" s="6" t="s">
         <v>598</v>
       </c>
@@ -11304,7 +11357,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C27" s="6" t="s">
         <v>600</v>
       </c>
@@ -11312,7 +11365,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
         <v>602</v>
       </c>
@@ -11323,7 +11376,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C29" s="6">
         <v>1</v>
       </c>
@@ -11345,17 +11398,17 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="9"/>
-    <col min="5" max="5" width="42.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="9"/>
+    <col min="5" max="5" width="42.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>531</v>
       </c>
@@ -11375,7 +11428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>411</v>
       </c>
@@ -11392,7 +11445,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>418</v>
       </c>
@@ -11406,7 +11459,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>610</v>
       </c>
@@ -11423,7 +11476,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>530</v>
       </c>
@@ -11440,7 +11493,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>542</v>
       </c>
@@ -11454,7 +11507,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
         <v>545</v>
       </c>
@@ -11464,34 +11517,34 @@
       <c r="D7" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="24" t="s">
         <v>621</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="22" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" s="9" t="s">
         <v>617</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="20"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="24"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" s="9" t="s">
         <v>618</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="20"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E9" s="24"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>540</v>
       </c>
@@ -11508,7 +11561,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>556</v>
       </c>
@@ -11528,7 +11581,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
         <v>572</v>
       </c>
@@ -11545,7 +11598,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
         <v>573</v>
       </c>
@@ -11562,7 +11615,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>629</v>
       </c>
@@ -11575,28 +11628,28 @@
       <c r="D14" s="9" t="s">
         <v>619</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="24" t="s">
         <v>632</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="22" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" s="9" t="s">
         <v>631</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>619</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="20"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E16" s="22"/>
-      <c r="F16" s="20"/>
-    </row>
-    <row r="17" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E15" s="24"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="24"/>
+      <c r="F16" s="22"/>
+    </row>
+    <row r="17" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
         <v>633</v>
       </c>
@@ -11613,7 +11666,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
         <v>635</v>
       </c>
@@ -11627,7 +11680,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="9" t="s">
         <v>602</v>
       </c>
@@ -11641,7 +11694,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
         <v>639</v>
       </c>
@@ -11655,7 +11708,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
         <v>642</v>
       </c>
@@ -11669,7 +11722,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>645</v>
       </c>
@@ -11683,7 +11736,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
         <v>648</v>
       </c>
@@ -11697,7 +11750,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
         <v>651</v>
       </c>
@@ -11714,7 +11767,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="9" t="s">
         <v>580</v>
       </c>
@@ -11724,24 +11777,24 @@
       <c r="D25" s="9" t="s">
         <v>517</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="24" t="s">
         <v>654</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="22" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C26" s="9" t="s">
         <v>640</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>517</v>
       </c>
-      <c r="E26" s="22"/>
-      <c r="F26" s="20"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="24"/>
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="9" t="s">
         <v>655</v>
       </c>
@@ -11751,32 +11804,32 @@
       <c r="D27" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="24" t="s">
         <v>657</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="22" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C28" s="9" t="s">
         <v>617</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E28" s="22"/>
-      <c r="F28" s="20"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="24"/>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C29" s="9" t="s">
         <v>656</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>611</v>
       </c>
-      <c r="E29" s="22"/>
-      <c r="F29" s="20"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>